<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@e03e131c338e4cfc0432bc2ad82e41e3c46f38bd 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -28082,7 +28082,7 @@
         </is>
       </c>
       <c r="B1012" t="n">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="C1012" t="inlineStr">
         <is>
@@ -28654,7 +28654,7 @@
         </is>
       </c>
       <c r="B1034" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1034" t="inlineStr">
         <is>
@@ -28680,7 +28680,7 @@
         </is>
       </c>
       <c r="B1035" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C1035" t="inlineStr">
         <is>
@@ -29798,7 +29798,7 @@
         </is>
       </c>
       <c r="B1078" t="n">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="C1078" t="inlineStr">
         <is>
@@ -30812,7 +30812,7 @@
         </is>
       </c>
       <c r="B1117" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1117" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@0d7eee55e3971f0da1ba64aab0924bb60a7351c4 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@f5821031d535e89823aed669582a40b3474ed1a3 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@f87b03cd6ede74a1e5ed3bbb24f6f58bf6cd24ec 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -5333,7 +5333,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
@@ -10709,7 +10709,7 @@
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
@@ -13873,7 +13873,7 @@
       </c>
       <c r="F480" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
@@ -18913,7 +18913,7 @@
       </c>
       <c r="F660" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
@@ -24233,7 +24233,7 @@
       </c>
       <c r="F850" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
@@ -31053,7 +31053,7 @@
       </c>
       <c r="F1111" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
@@ -35863,7 +35863,7 @@
       </c>
       <c r="F1296" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
@@ -37579,7 +37579,7 @@
       </c>
       <c r="F1362" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@72b66f057ad5250541efdb4ba3809949d0b185b9 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@815531674ad2caa6ebc64b61b786dbe449cfb3dd 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1519"/>
+  <dimension ref="A1:F1518"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31916,7 +31916,7 @@
         </is>
       </c>
       <c r="B1144" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1144" t="inlineStr">
         <is>
@@ -31968,7 +31968,7 @@
         </is>
       </c>
       <c r="B1146" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1146" t="inlineStr">
         <is>
@@ -31994,7 +31994,7 @@
         </is>
       </c>
       <c r="B1147" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1147" t="inlineStr">
         <is>
@@ -32046,7 +32046,7 @@
         </is>
       </c>
       <c r="B1149" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1149" t="inlineStr">
         <is>
@@ -32124,7 +32124,7 @@
         </is>
       </c>
       <c r="B1152" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1152" t="inlineStr">
         <is>
@@ -32228,7 +32228,7 @@
         </is>
       </c>
       <c r="B1156" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1156" t="inlineStr">
         <is>
@@ -32332,7 +32332,7 @@
         </is>
       </c>
       <c r="B1160" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1160" t="inlineStr">
         <is>
@@ -32358,7 +32358,7 @@
         </is>
       </c>
       <c r="B1161" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1161" t="inlineStr">
         <is>
@@ -32462,7 +32462,7 @@
         </is>
       </c>
       <c r="B1165" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C1165" t="inlineStr">
         <is>
@@ -32670,7 +32670,7 @@
         </is>
       </c>
       <c r="B1173" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1173" t="inlineStr">
         <is>
@@ -32748,7 +32748,7 @@
         </is>
       </c>
       <c r="B1176" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1176" t="inlineStr">
         <is>
@@ -32774,7 +32774,7 @@
         </is>
       </c>
       <c r="B1177" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1177" t="inlineStr">
         <is>
@@ -32800,7 +32800,7 @@
         </is>
       </c>
       <c r="B1178" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1178" t="inlineStr">
         <is>
@@ -32826,7 +32826,7 @@
         </is>
       </c>
       <c r="B1179" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1179" t="inlineStr">
         <is>
@@ -32878,7 +32878,7 @@
         </is>
       </c>
       <c r="B1181" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1181" t="inlineStr">
         <is>
@@ -32904,7 +32904,7 @@
         </is>
       </c>
       <c r="B1182" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1182" t="inlineStr">
         <is>
@@ -32982,7 +32982,7 @@
         </is>
       </c>
       <c r="B1185" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1185" t="inlineStr">
         <is>
@@ -33008,7 +33008,7 @@
         </is>
       </c>
       <c r="B1186" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1186" t="inlineStr">
         <is>
@@ -33034,7 +33034,7 @@
         </is>
       </c>
       <c r="B1187" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C1187" t="inlineStr">
         <is>
@@ -33060,7 +33060,7 @@
         </is>
       </c>
       <c r="B1188" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1188" t="inlineStr">
         <is>
@@ -33086,7 +33086,7 @@
         </is>
       </c>
       <c r="B1189" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1189" t="inlineStr">
         <is>
@@ -33164,7 +33164,7 @@
         </is>
       </c>
       <c r="B1192" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1192" t="inlineStr">
         <is>
@@ -33216,7 +33216,7 @@
         </is>
       </c>
       <c r="B1194" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C1194" t="inlineStr">
         <is>
@@ -33294,7 +33294,7 @@
         </is>
       </c>
       <c r="B1197" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="C1197" t="inlineStr">
         <is>
@@ -33320,7 +33320,7 @@
         </is>
       </c>
       <c r="B1198" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1198" t="inlineStr">
         <is>
@@ -33398,7 +33398,7 @@
         </is>
       </c>
       <c r="B1201" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="C1201" t="inlineStr">
         <is>
@@ -33450,7 +33450,7 @@
         </is>
       </c>
       <c r="B1203" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1203" t="inlineStr">
         <is>
@@ -33528,7 +33528,7 @@
         </is>
       </c>
       <c r="B1206" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1206" t="inlineStr">
         <is>
@@ -33580,7 +33580,7 @@
         </is>
       </c>
       <c r="B1208" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1208" t="inlineStr">
         <is>
@@ -33632,7 +33632,7 @@
         </is>
       </c>
       <c r="B1210" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1210" t="inlineStr">
         <is>
@@ -33684,7 +33684,7 @@
         </is>
       </c>
       <c r="B1212" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1212" t="inlineStr">
         <is>
@@ -33736,7 +33736,7 @@
         </is>
       </c>
       <c r="B1214" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C1214" t="inlineStr">
         <is>
@@ -33866,7 +33866,7 @@
         </is>
       </c>
       <c r="B1219" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C1219" t="inlineStr">
         <is>
@@ -34204,7 +34204,7 @@
         </is>
       </c>
       <c r="B1232" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1232" t="inlineStr">
         <is>
@@ -34230,7 +34230,7 @@
         </is>
       </c>
       <c r="B1233" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C1233" t="inlineStr">
         <is>
@@ -34256,7 +34256,7 @@
         </is>
       </c>
       <c r="B1234" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="C1234" t="inlineStr">
         <is>
@@ -34360,7 +34360,7 @@
         </is>
       </c>
       <c r="B1238" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1238" t="inlineStr">
         <is>
@@ -34386,7 +34386,7 @@
         </is>
       </c>
       <c r="B1239" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1239" t="inlineStr">
         <is>
@@ -34412,7 +34412,7 @@
         </is>
       </c>
       <c r="B1240" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1240" t="inlineStr">
         <is>
@@ -34464,7 +34464,7 @@
         </is>
       </c>
       <c r="B1242" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1242" t="inlineStr">
         <is>
@@ -34620,7 +34620,7 @@
         </is>
       </c>
       <c r="B1248" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1248" t="inlineStr">
         <is>
@@ -34672,7 +34672,7 @@
         </is>
       </c>
       <c r="B1250" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1250" t="inlineStr">
         <is>
@@ -34880,7 +34880,7 @@
         </is>
       </c>
       <c r="B1258" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="C1258" t="inlineStr">
         <is>
@@ -35010,7 +35010,7 @@
         </is>
       </c>
       <c r="B1263" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1263" t="inlineStr">
         <is>
@@ -35140,7 +35140,7 @@
         </is>
       </c>
       <c r="B1268" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1268" t="inlineStr">
         <is>
@@ -35166,7 +35166,7 @@
         </is>
       </c>
       <c r="B1269" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1269" t="inlineStr">
         <is>
@@ -35192,7 +35192,7 @@
         </is>
       </c>
       <c r="B1270" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C1270" t="inlineStr">
         <is>
@@ -35244,7 +35244,7 @@
         </is>
       </c>
       <c r="B1272" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1272" t="inlineStr">
         <is>
@@ -35270,7 +35270,7 @@
         </is>
       </c>
       <c r="B1273" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1273" t="inlineStr">
         <is>
@@ -35296,7 +35296,7 @@
         </is>
       </c>
       <c r="B1274" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1274" t="inlineStr">
         <is>
@@ -35348,7 +35348,7 @@
         </is>
       </c>
       <c r="B1276" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1276" t="inlineStr">
         <is>
@@ -35556,7 +35556,7 @@
         </is>
       </c>
       <c r="B1284" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1284" t="inlineStr">
         <is>
@@ -35578,11 +35578,11 @@
     <row r="1285">
       <c r="A1285" t="inlineStr">
         <is>
-          <t>SOM</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="B1285" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="C1285" t="inlineStr">
         <is>
@@ -35597,18 +35597,18 @@
       </c>
       <c r="F1285" t="inlineStr">
         <is>
-          <t>Somalia</t>
+          <t>Serbia</t>
         </is>
       </c>
     </row>
     <row r="1286">
       <c r="A1286" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="B1286" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="C1286" t="inlineStr">
         <is>
@@ -35623,18 +35623,18 @@
       </c>
       <c r="F1286" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>South Sudan</t>
         </is>
       </c>
     </row>
     <row r="1287">
       <c r="A1287" t="inlineStr">
         <is>
-          <t>SSD</t>
+          <t>SSF</t>
         </is>
       </c>
       <c r="B1287" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="C1287" t="inlineStr">
         <is>
@@ -35649,18 +35649,18 @@
       </c>
       <c r="F1287" t="inlineStr">
         <is>
-          <t>South Sudan</t>
+          <t>SSF</t>
         </is>
       </c>
     </row>
     <row r="1288">
       <c r="A1288" t="inlineStr">
         <is>
-          <t>SSF</t>
+          <t>STP</t>
         </is>
       </c>
       <c r="B1288" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C1288" t="inlineStr">
         <is>
@@ -35675,18 +35675,18 @@
       </c>
       <c r="F1288" t="inlineStr">
         <is>
-          <t>SSF</t>
+          <t>Sao Tome and Principe</t>
         </is>
       </c>
     </row>
     <row r="1289">
       <c r="A1289" t="inlineStr">
         <is>
-          <t>STP</t>
+          <t>SUR</t>
         </is>
       </c>
       <c r="B1289" t="n">
-        <v>2017</v>
+        <v>1999</v>
       </c>
       <c r="C1289" t="inlineStr">
         <is>
@@ -35701,18 +35701,18 @@
       </c>
       <c r="F1289" t="inlineStr">
         <is>
-          <t>Sao Tome and Principe</t>
+          <t>Suriname</t>
         </is>
       </c>
     </row>
     <row r="1290">
       <c r="A1290" t="inlineStr">
         <is>
-          <t>SUR</t>
+          <t>SVK</t>
         </is>
       </c>
       <c r="B1290" t="n">
-        <v>1999</v>
+        <v>2019</v>
       </c>
       <c r="C1290" t="inlineStr">
         <is>
@@ -35727,18 +35727,18 @@
       </c>
       <c r="F1290" t="inlineStr">
         <is>
-          <t>Suriname</t>
+          <t>Slovakia</t>
         </is>
       </c>
     </row>
     <row r="1291">
       <c r="A1291" t="inlineStr">
         <is>
-          <t>SVK</t>
+          <t>SVN</t>
         </is>
       </c>
       <c r="B1291" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1291" t="inlineStr">
         <is>
@@ -35753,18 +35753,18 @@
       </c>
       <c r="F1291" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Slovenia</t>
         </is>
       </c>
     </row>
     <row r="1292">
       <c r="A1292" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>SWE</t>
         </is>
       </c>
       <c r="B1292" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1292" t="inlineStr">
         <is>
@@ -35779,18 +35779,18 @@
       </c>
       <c r="F1292" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Sweden</t>
         </is>
       </c>
     </row>
     <row r="1293">
       <c r="A1293" t="inlineStr">
         <is>
-          <t>SWE</t>
+          <t>SWZ</t>
         </is>
       </c>
       <c r="B1293" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="C1293" t="inlineStr">
         <is>
@@ -35805,18 +35805,18 @@
       </c>
       <c r="F1293" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Eswatini</t>
         </is>
       </c>
     </row>
     <row r="1294">
       <c r="A1294" t="inlineStr">
         <is>
-          <t>SWZ</t>
+          <t>SYC</t>
         </is>
       </c>
       <c r="B1294" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="C1294" t="inlineStr">
         <is>
@@ -35831,18 +35831,18 @@
       </c>
       <c r="F1294" t="inlineStr">
         <is>
-          <t>Eswatini</t>
+          <t>Seychelles</t>
         </is>
       </c>
     </row>
     <row r="1295">
       <c r="A1295" t="inlineStr">
         <is>
-          <t>SYC</t>
+          <t>SYR</t>
         </is>
       </c>
       <c r="B1295" t="n">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="C1295" t="inlineStr">
         <is>
@@ -35857,18 +35857,18 @@
       </c>
       <c r="F1295" t="inlineStr">
         <is>
-          <t>Seychelles</t>
+          <t>Syria</t>
         </is>
       </c>
     </row>
     <row r="1296">
       <c r="A1296" t="inlineStr">
         <is>
-          <t>SYR</t>
+          <t>TCD</t>
         </is>
       </c>
       <c r="B1296" t="n">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="C1296" t="inlineStr">
         <is>
@@ -35883,14 +35883,14 @@
       </c>
       <c r="F1296" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Chad</t>
         </is>
       </c>
     </row>
     <row r="1297">
       <c r="A1297" t="inlineStr">
         <is>
-          <t>TCD</t>
+          <t>TGO</t>
         </is>
       </c>
       <c r="B1297" t="n">
@@ -35909,18 +35909,18 @@
       </c>
       <c r="F1297" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>Togo</t>
         </is>
       </c>
     </row>
     <row r="1298">
       <c r="A1298" t="inlineStr">
         <is>
-          <t>TGO</t>
+          <t>THA</t>
         </is>
       </c>
       <c r="B1298" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C1298" t="inlineStr">
         <is>
@@ -35935,18 +35935,18 @@
       </c>
       <c r="F1298" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Thailand</t>
         </is>
       </c>
     </row>
     <row r="1299">
       <c r="A1299" t="inlineStr">
         <is>
-          <t>THA</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="B1299" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="C1299" t="inlineStr">
         <is>
@@ -35961,18 +35961,18 @@
       </c>
       <c r="F1299" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Tajikistan</t>
         </is>
       </c>
     </row>
     <row r="1300">
       <c r="A1300" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="B1300" t="n">
-        <v>2015</v>
+        <v>1998</v>
       </c>
       <c r="C1300" t="inlineStr">
         <is>
@@ -35987,18 +35987,18 @@
       </c>
       <c r="F1300" t="inlineStr">
         <is>
-          <t>Tajikistan</t>
+          <t>Turkmenistan</t>
         </is>
       </c>
     </row>
     <row r="1301">
       <c r="A1301" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>TLS</t>
         </is>
       </c>
       <c r="B1301" t="n">
-        <v>1998</v>
+        <v>2014</v>
       </c>
       <c r="C1301" t="inlineStr">
         <is>
@@ -36013,18 +36013,18 @@
       </c>
       <c r="F1301" t="inlineStr">
         <is>
-          <t>Turkmenistan</t>
+          <t>Timor-Leste</t>
         </is>
       </c>
     </row>
     <row r="1302">
       <c r="A1302" t="inlineStr">
         <is>
-          <t>TLS</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="B1302" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="C1302" t="inlineStr">
         <is>
@@ -36039,18 +36039,18 @@
       </c>
       <c r="F1302" t="inlineStr">
         <is>
-          <t>Timor-Leste</t>
+          <t>Tonga</t>
         </is>
       </c>
     </row>
     <row r="1303">
       <c r="A1303" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>TTO</t>
         </is>
       </c>
       <c r="B1303" t="n">
-        <v>2015</v>
+        <v>1992</v>
       </c>
       <c r="C1303" t="inlineStr">
         <is>
@@ -36065,18 +36065,18 @@
       </c>
       <c r="F1303" t="inlineStr">
         <is>
-          <t>Tonga</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
     </row>
     <row r="1304">
       <c r="A1304" t="inlineStr">
         <is>
-          <t>TTO</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="B1304" t="n">
-        <v>1992</v>
+        <v>2015</v>
       </c>
       <c r="C1304" t="inlineStr">
         <is>
@@ -36091,18 +36091,18 @@
       </c>
       <c r="F1304" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Tunisia</t>
         </is>
       </c>
     </row>
     <row r="1305">
       <c r="A1305" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>TUR</t>
         </is>
       </c>
       <c r="B1305" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="C1305" t="inlineStr">
         <is>
@@ -36117,18 +36117,18 @@
       </c>
       <c r="F1305" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
     <row r="1306">
       <c r="A1306" t="inlineStr">
         <is>
-          <t>TUR</t>
+          <t>TUV</t>
         </is>
       </c>
       <c r="B1306" t="n">
-        <v>2019</v>
+        <v>2010</v>
       </c>
       <c r="C1306" t="inlineStr">
         <is>
@@ -36143,18 +36143,18 @@
       </c>
       <c r="F1306" t="inlineStr">
         <is>
-          <t>Türkiye</t>
+          <t>Tuvalu</t>
         </is>
       </c>
     </row>
     <row r="1307">
       <c r="A1307" t="inlineStr">
         <is>
-          <t>TUV</t>
+          <t>TZA</t>
         </is>
       </c>
       <c r="B1307" t="n">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="C1307" t="inlineStr">
         <is>
@@ -36169,18 +36169,18 @@
       </c>
       <c r="F1307" t="inlineStr">
         <is>
-          <t>Tuvalu</t>
+          <t>Tanzania</t>
         </is>
       </c>
     </row>
     <row r="1308">
       <c r="A1308" t="inlineStr">
         <is>
-          <t>TZA</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="B1308" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1308" t="inlineStr">
         <is>
@@ -36195,18 +36195,18 @@
       </c>
       <c r="F1308" t="inlineStr">
         <is>
-          <t>Tanzania</t>
+          <t>Uganda</t>
         </is>
       </c>
     </row>
     <row r="1309">
       <c r="A1309" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="B1309" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1309" t="inlineStr">
         <is>
@@ -36221,18 +36221,18 @@
       </c>
       <c r="F1309" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Ukraine</t>
         </is>
       </c>
     </row>
     <row r="1310">
       <c r="A1310" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>UMC</t>
         </is>
       </c>
       <c r="B1310" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C1310" t="inlineStr">
         <is>
@@ -36247,18 +36247,18 @@
       </c>
       <c r="F1310" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>UMC</t>
         </is>
       </c>
     </row>
     <row r="1311">
       <c r="A1311" t="inlineStr">
         <is>
-          <t>UMC</t>
+          <t>URY</t>
         </is>
       </c>
       <c r="B1311" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1311" t="inlineStr">
         <is>
@@ -36273,14 +36273,14 @@
       </c>
       <c r="F1311" t="inlineStr">
         <is>
-          <t>UMC</t>
+          <t>Uruguay</t>
         </is>
       </c>
     </row>
     <row r="1312">
       <c r="A1312" t="inlineStr">
         <is>
-          <t>URY</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B1312" t="n">
@@ -36299,18 +36299,18 @@
       </c>
       <c r="F1312" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>United States</t>
         </is>
       </c>
     </row>
     <row r="1313">
       <c r="A1313" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="B1313" t="n">
-        <v>2019</v>
+        <v>2003</v>
       </c>
       <c r="C1313" t="inlineStr">
         <is>
@@ -36325,18 +36325,18 @@
       </c>
       <c r="F1313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Uzbekistan</t>
         </is>
       </c>
     </row>
     <row r="1314">
       <c r="A1314" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>VEN</t>
         </is>
       </c>
       <c r="B1314" t="n">
-        <v>2003</v>
+        <v>2006</v>
       </c>
       <c r="C1314" t="inlineStr">
         <is>
@@ -36351,18 +36351,18 @@
       </c>
       <c r="F1314" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Venezuela</t>
         </is>
       </c>
     </row>
     <row r="1315">
       <c r="A1315" t="inlineStr">
         <is>
-          <t>VEN</t>
+          <t>VNM</t>
         </is>
       </c>
       <c r="B1315" t="n">
-        <v>2006</v>
+        <v>2020</v>
       </c>
       <c r="C1315" t="inlineStr">
         <is>
@@ -36377,18 +36377,18 @@
       </c>
       <c r="F1315" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>Vietnam</t>
         </is>
       </c>
     </row>
     <row r="1316">
       <c r="A1316" t="inlineStr">
         <is>
-          <t>VNM</t>
+          <t>VUT</t>
         </is>
       </c>
       <c r="B1316" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1316" t="inlineStr">
         <is>
@@ -36403,14 +36403,14 @@
       </c>
       <c r="F1316" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Vanuatu</t>
         </is>
       </c>
     </row>
     <row r="1317">
       <c r="A1317" t="inlineStr">
         <is>
-          <t>VUT</t>
+          <t>WLD</t>
         </is>
       </c>
       <c r="B1317" t="n">
@@ -36429,18 +36429,18 @@
       </c>
       <c r="F1317" t="inlineStr">
         <is>
-          <t>Vanuatu</t>
+          <t>WLD</t>
         </is>
       </c>
     </row>
     <row r="1318">
       <c r="A1318" t="inlineStr">
         <is>
-          <t>WLD</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="B1318" t="n">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="C1318" t="inlineStr">
         <is>
@@ -36455,18 +36455,18 @@
       </c>
       <c r="F1318" t="inlineStr">
         <is>
-          <t>WLD</t>
+          <t>Samoa</t>
         </is>
       </c>
     </row>
     <row r="1319">
       <c r="A1319" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>XKX</t>
         </is>
       </c>
       <c r="B1319" t="n">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="C1319" t="inlineStr">
         <is>
@@ -36481,18 +36481,18 @@
       </c>
       <c r="F1319" t="inlineStr">
         <is>
-          <t>Samoa</t>
+          <t>Kosovo</t>
         </is>
       </c>
     </row>
     <row r="1320">
       <c r="A1320" t="inlineStr">
         <is>
-          <t>XKX</t>
+          <t>YEM</t>
         </is>
       </c>
       <c r="B1320" t="n">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="C1320" t="inlineStr">
         <is>
@@ -36507,14 +36507,14 @@
       </c>
       <c r="F1320" t="inlineStr">
         <is>
-          <t>Kosovo</t>
+          <t>Yemen</t>
         </is>
       </c>
     </row>
     <row r="1321">
       <c r="A1321" t="inlineStr">
         <is>
-          <t>YEM</t>
+          <t>ZAF</t>
         </is>
       </c>
       <c r="B1321" t="n">
@@ -36533,18 +36533,18 @@
       </c>
       <c r="F1321" t="inlineStr">
         <is>
-          <t>Yemen</t>
+          <t>South Africa</t>
         </is>
       </c>
     </row>
     <row r="1322">
       <c r="A1322" t="inlineStr">
         <is>
-          <t>ZAF</t>
+          <t>ZMB</t>
         </is>
       </c>
       <c r="B1322" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="C1322" t="inlineStr">
         <is>
@@ -36559,18 +36559,18 @@
       </c>
       <c r="F1322" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Zambia</t>
         </is>
       </c>
     </row>
     <row r="1323">
       <c r="A1323" t="inlineStr">
         <is>
-          <t>ZMB</t>
+          <t>ZWE</t>
         </is>
       </c>
       <c r="B1323" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="C1323" t="inlineStr">
         <is>
@@ -36585,40 +36585,40 @@
       </c>
       <c r="F1323" t="inlineStr">
         <is>
-          <t>Zambia</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
     </row>
     <row r="1324">
       <c r="A1324" t="inlineStr">
         <is>
-          <t>ZWE</t>
+          <t>CHE</t>
         </is>
       </c>
       <c r="B1324" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1324" t="inlineStr">
         <is>
-          <t>Poverty rate (%)</t>
+          <t>Human Development Index</t>
         </is>
       </c>
       <c r="D1324" t="inlineStr"/>
       <c r="E1324" t="inlineStr">
         <is>
-          <t>World Bank Open Data</t>
+          <t>UNDP Human Development Report</t>
         </is>
       </c>
       <c r="F1324" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>Switzerland</t>
         </is>
       </c>
     </row>
     <row r="1325">
       <c r="A1325" t="inlineStr">
         <is>
-          <t>CHE</t>
+          <t>NOR</t>
         </is>
       </c>
       <c r="B1325" t="n">
@@ -36637,14 +36637,14 @@
       </c>
       <c r="F1325" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Norway</t>
         </is>
       </c>
     </row>
     <row r="1326">
       <c r="A1326" t="inlineStr">
         <is>
-          <t>NOR</t>
+          <t>ISL</t>
         </is>
       </c>
       <c r="B1326" t="n">
@@ -36663,14 +36663,14 @@
       </c>
       <c r="F1326" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Iceland</t>
         </is>
       </c>
     </row>
     <row r="1327">
       <c r="A1327" t="inlineStr">
         <is>
-          <t>ISL</t>
+          <t>HKG</t>
         </is>
       </c>
       <c r="B1327" t="n">
@@ -36689,14 +36689,14 @@
       </c>
       <c r="F1327" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Hong Kong</t>
         </is>
       </c>
     </row>
     <row r="1328">
       <c r="A1328" t="inlineStr">
         <is>
-          <t>HKG</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B1328" t="n">
@@ -36715,14 +36715,14 @@
       </c>
       <c r="F1328" t="inlineStr">
         <is>
-          <t>Hong Kong</t>
+          <t>Australia</t>
         </is>
       </c>
     </row>
     <row r="1329">
       <c r="A1329" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>DNK</t>
         </is>
       </c>
       <c r="B1329" t="n">
@@ -36741,14 +36741,14 @@
       </c>
       <c r="F1329" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Denmark</t>
         </is>
       </c>
     </row>
     <row r="1330">
       <c r="A1330" t="inlineStr">
         <is>
-          <t>DNK</t>
+          <t>SWE</t>
         </is>
       </c>
       <c r="B1330" t="n">
@@ -36767,14 +36767,14 @@
       </c>
       <c r="F1330" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Sweden</t>
         </is>
       </c>
     </row>
     <row r="1331">
       <c r="A1331" t="inlineStr">
         <is>
-          <t>SWE</t>
+          <t>IRL</t>
         </is>
       </c>
       <c r="B1331" t="n">
@@ -36793,14 +36793,14 @@
       </c>
       <c r="F1331" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Ireland</t>
         </is>
       </c>
     </row>
     <row r="1332">
       <c r="A1332" t="inlineStr">
         <is>
-          <t>IRL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="B1332" t="n">
@@ -36819,14 +36819,14 @@
       </c>
       <c r="F1332" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Germany</t>
         </is>
       </c>
     </row>
     <row r="1333">
       <c r="A1333" t="inlineStr">
         <is>
-          <t>DEU</t>
+          <t>NLD</t>
         </is>
       </c>
       <c r="B1333" t="n">
@@ -36845,14 +36845,14 @@
       </c>
       <c r="F1333" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
     <row r="1334">
       <c r="A1334" t="inlineStr">
         <is>
-          <t>NLD</t>
+          <t>FIN</t>
         </is>
       </c>
       <c r="B1334" t="n">
@@ -36871,14 +36871,14 @@
       </c>
       <c r="F1334" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Finland</t>
         </is>
       </c>
     </row>
     <row r="1335">
       <c r="A1335" t="inlineStr">
         <is>
-          <t>FIN</t>
+          <t>SGP</t>
         </is>
       </c>
       <c r="B1335" t="n">
@@ -36897,14 +36897,14 @@
       </c>
       <c r="F1335" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Singapore</t>
         </is>
       </c>
     </row>
     <row r="1336">
       <c r="A1336" t="inlineStr">
         <is>
-          <t>SGP</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B1336" t="n">
@@ -36923,14 +36923,14 @@
       </c>
       <c r="F1336" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Belgium</t>
         </is>
       </c>
     </row>
     <row r="1337">
       <c r="A1337" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>NZL</t>
         </is>
       </c>
       <c r="B1337" t="n">
@@ -36949,14 +36949,14 @@
       </c>
       <c r="F1337" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>New Zealand</t>
         </is>
       </c>
     </row>
     <row r="1338">
       <c r="A1338" t="inlineStr">
         <is>
-          <t>NZL</t>
+          <t>CAN</t>
         </is>
       </c>
       <c r="B1338" t="n">
@@ -36975,14 +36975,14 @@
       </c>
       <c r="F1338" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Canada</t>
         </is>
       </c>
     </row>
     <row r="1339">
       <c r="A1339" t="inlineStr">
         <is>
-          <t>CAN</t>
+          <t>LIE</t>
         </is>
       </c>
       <c r="B1339" t="n">
@@ -37001,14 +37001,14 @@
       </c>
       <c r="F1339" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Liechtenstein</t>
         </is>
       </c>
     </row>
     <row r="1340">
       <c r="A1340" t="inlineStr">
         <is>
-          <t>LIE</t>
+          <t>LUX</t>
         </is>
       </c>
       <c r="B1340" t="n">
@@ -37027,14 +37027,14 @@
       </c>
       <c r="F1340" t="inlineStr">
         <is>
-          <t>Liechtenstein</t>
+          <t>Luxembourg</t>
         </is>
       </c>
     </row>
     <row r="1341">
       <c r="A1341" t="inlineStr">
         <is>
-          <t>LUX</t>
+          <t>GBR</t>
         </is>
       </c>
       <c r="B1341" t="n">
@@ -37053,14 +37053,14 @@
       </c>
       <c r="F1341" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>United Kingdom</t>
         </is>
       </c>
     </row>
     <row r="1342">
       <c r="A1342" t="inlineStr">
         <is>
-          <t>GBR</t>
+          <t>JPN</t>
         </is>
       </c>
       <c r="B1342" t="n">
@@ -37079,14 +37079,14 @@
       </c>
       <c r="F1342" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Japan</t>
         </is>
       </c>
     </row>
     <row r="1343">
       <c r="A1343" t="inlineStr">
         <is>
-          <t>JPN</t>
+          <t>KOR</t>
         </is>
       </c>
       <c r="B1343" t="n">
@@ -37105,14 +37105,14 @@
       </c>
       <c r="F1343" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>South Korea</t>
         </is>
       </c>
     </row>
     <row r="1344">
       <c r="A1344" t="inlineStr">
         <is>
-          <t>KOR</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B1344" t="n">
@@ -37131,14 +37131,14 @@
       </c>
       <c r="F1344" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>United States</t>
         </is>
       </c>
     </row>
     <row r="1345">
       <c r="A1345" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>ISR</t>
         </is>
       </c>
       <c r="B1345" t="n">
@@ -37157,14 +37157,14 @@
       </c>
       <c r="F1345" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Israel</t>
         </is>
       </c>
     </row>
     <row r="1346">
       <c r="A1346" t="inlineStr">
         <is>
-          <t>ISR</t>
+          <t>MLT</t>
         </is>
       </c>
       <c r="B1346" t="n">
@@ -37183,14 +37183,14 @@
       </c>
       <c r="F1346" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Malta</t>
         </is>
       </c>
     </row>
     <row r="1347">
       <c r="A1347" t="inlineStr">
         <is>
-          <t>MLT</t>
+          <t>SVN</t>
         </is>
       </c>
       <c r="B1347" t="n">
@@ -37209,14 +37209,14 @@
       </c>
       <c r="F1347" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Slovenia</t>
         </is>
       </c>
     </row>
     <row r="1348">
       <c r="A1348" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>AUT</t>
         </is>
       </c>
       <c r="B1348" t="n">
@@ -37235,14 +37235,14 @@
       </c>
       <c r="F1348" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Austria</t>
         </is>
       </c>
     </row>
     <row r="1349">
       <c r="A1349" t="inlineStr">
         <is>
-          <t>AUT</t>
+          <t>ARE</t>
         </is>
       </c>
       <c r="B1349" t="n">
@@ -37261,14 +37261,14 @@
       </c>
       <c r="F1349" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>United Arab Emirates</t>
         </is>
       </c>
     </row>
     <row r="1350">
       <c r="A1350" t="inlineStr">
         <is>
-          <t>ARE</t>
+          <t>ESP</t>
         </is>
       </c>
       <c r="B1350" t="n">
@@ -37287,14 +37287,14 @@
       </c>
       <c r="F1350" t="inlineStr">
         <is>
-          <t>United Arab Emirates</t>
+          <t>Spain</t>
         </is>
       </c>
     </row>
     <row r="1351">
       <c r="A1351" t="inlineStr">
         <is>
-          <t>ESP</t>
+          <t>FRA</t>
         </is>
       </c>
       <c r="B1351" t="n">
@@ -37313,14 +37313,14 @@
       </c>
       <c r="F1351" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>France</t>
         </is>
       </c>
     </row>
     <row r="1352">
       <c r="A1352" t="inlineStr">
         <is>
-          <t>FRA</t>
+          <t>CYP</t>
         </is>
       </c>
       <c r="B1352" t="n">
@@ -37339,14 +37339,14 @@
       </c>
       <c r="F1352" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Cyprus</t>
         </is>
       </c>
     </row>
     <row r="1353">
       <c r="A1353" t="inlineStr">
         <is>
-          <t>CYP</t>
+          <t>ITA</t>
         </is>
       </c>
       <c r="B1353" t="n">
@@ -37365,14 +37365,14 @@
       </c>
       <c r="F1353" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Italy</t>
         </is>
       </c>
     </row>
     <row r="1354">
       <c r="A1354" t="inlineStr">
         <is>
-          <t>ITA</t>
+          <t>EST</t>
         </is>
       </c>
       <c r="B1354" t="n">
@@ -37391,14 +37391,14 @@
       </c>
       <c r="F1354" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Estonia</t>
         </is>
       </c>
     </row>
     <row r="1355">
       <c r="A1355" t="inlineStr">
         <is>
-          <t>EST</t>
+          <t>CZE</t>
         </is>
       </c>
       <c r="B1355" t="n">
@@ -37417,14 +37417,14 @@
       </c>
       <c r="F1355" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>Czech Republic</t>
         </is>
       </c>
     </row>
     <row r="1356">
       <c r="A1356" t="inlineStr">
         <is>
-          <t>CZE</t>
+          <t>GRC</t>
         </is>
       </c>
       <c r="B1356" t="n">
@@ -37443,14 +37443,14 @@
       </c>
       <c r="F1356" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Greece</t>
         </is>
       </c>
     </row>
     <row r="1357">
       <c r="A1357" t="inlineStr">
         <is>
-          <t>GRC</t>
+          <t>POL</t>
         </is>
       </c>
       <c r="B1357" t="n">
@@ -37469,14 +37469,14 @@
       </c>
       <c r="F1357" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Poland</t>
         </is>
       </c>
     </row>
     <row r="1358">
       <c r="A1358" t="inlineStr">
         <is>
-          <t>POL</t>
+          <t>BHR</t>
         </is>
       </c>
       <c r="B1358" t="n">
@@ -37495,14 +37495,14 @@
       </c>
       <c r="F1358" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Bahrain</t>
         </is>
       </c>
     </row>
     <row r="1359">
       <c r="A1359" t="inlineStr">
         <is>
-          <t>BHR</t>
+          <t>LTU</t>
         </is>
       </c>
       <c r="B1359" t="n">
@@ -37521,14 +37521,14 @@
       </c>
       <c r="F1359" t="inlineStr">
         <is>
-          <t>Bahrain</t>
+          <t>Lithuania</t>
         </is>
       </c>
     </row>
     <row r="1360">
       <c r="A1360" t="inlineStr">
         <is>
-          <t>LTU</t>
+          <t>SAU</t>
         </is>
       </c>
       <c r="B1360" t="n">
@@ -37547,14 +37547,14 @@
       </c>
       <c r="F1360" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
     </row>
     <row r="1361">
       <c r="A1361" t="inlineStr">
         <is>
-          <t>SAU</t>
+          <t>PRT</t>
         </is>
       </c>
       <c r="B1361" t="n">
@@ -37573,14 +37573,14 @@
       </c>
       <c r="F1361" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>Portugal</t>
         </is>
       </c>
     </row>
     <row r="1362">
       <c r="A1362" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>LVA</t>
         </is>
       </c>
       <c r="B1362" t="n">
@@ -37599,14 +37599,14 @@
       </c>
       <c r="F1362" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Latvia</t>
         </is>
       </c>
     </row>
     <row r="1363">
       <c r="A1363" t="inlineStr">
         <is>
-          <t>LVA</t>
+          <t>AND</t>
         </is>
       </c>
       <c r="B1363" t="n">
@@ -37625,14 +37625,14 @@
       </c>
       <c r="F1363" t="inlineStr">
         <is>
-          <t>Latvia</t>
+          <t>Andorra</t>
         </is>
       </c>
     </row>
     <row r="1364">
       <c r="A1364" t="inlineStr">
         <is>
-          <t>AND</t>
+          <t>HRV</t>
         </is>
       </c>
       <c r="B1364" t="n">
@@ -37651,14 +37651,14 @@
       </c>
       <c r="F1364" t="inlineStr">
         <is>
-          <t>Andorra</t>
+          <t>Croatia</t>
         </is>
       </c>
     </row>
     <row r="1365">
       <c r="A1365" t="inlineStr">
         <is>
-          <t>HRV</t>
+          <t>CHL</t>
         </is>
       </c>
       <c r="B1365" t="n">
@@ -37677,14 +37677,14 @@
       </c>
       <c r="F1365" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Chile</t>
         </is>
       </c>
     </row>
     <row r="1366">
       <c r="A1366" t="inlineStr">
         <is>
-          <t>CHL</t>
+          <t>QAT</t>
         </is>
       </c>
       <c r="B1366" t="n">
@@ -37703,14 +37703,14 @@
       </c>
       <c r="F1366" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Qatar</t>
         </is>
       </c>
     </row>
     <row r="1367">
       <c r="A1367" t="inlineStr">
         <is>
-          <t>QAT</t>
+          <t>SMR</t>
         </is>
       </c>
       <c r="B1367" t="n">
@@ -37729,14 +37729,14 @@
       </c>
       <c r="F1367" t="inlineStr">
         <is>
-          <t>Qatar</t>
+          <t>San Marino</t>
         </is>
       </c>
     </row>
     <row r="1368">
       <c r="A1368" t="inlineStr">
         <is>
-          <t>SMR</t>
+          <t>SVK</t>
         </is>
       </c>
       <c r="B1368" t="n">
@@ -37755,14 +37755,14 @@
       </c>
       <c r="F1368" t="inlineStr">
         <is>
-          <t>San Marino</t>
+          <t>Slovakia</t>
         </is>
       </c>
     </row>
     <row r="1369">
       <c r="A1369" t="inlineStr">
         <is>
-          <t>SVK</t>
+          <t>HUN</t>
         </is>
       </c>
       <c r="B1369" t="n">
@@ -37781,14 +37781,14 @@
       </c>
       <c r="F1369" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Hungary</t>
         </is>
       </c>
     </row>
     <row r="1370">
       <c r="A1370" t="inlineStr">
         <is>
-          <t>HUN</t>
+          <t>ARG</t>
         </is>
       </c>
       <c r="B1370" t="n">
@@ -37807,14 +37807,14 @@
       </c>
       <c r="F1370" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Argentina</t>
         </is>
       </c>
     </row>
     <row r="1371">
       <c r="A1371" t="inlineStr">
         <is>
-          <t>ARG</t>
+          <t>TUR</t>
         </is>
       </c>
       <c r="B1371" t="n">
@@ -37833,14 +37833,14 @@
       </c>
       <c r="F1371" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Türkiye</t>
         </is>
       </c>
     </row>
     <row r="1372">
       <c r="A1372" t="inlineStr">
         <is>
-          <t>TUR</t>
+          <t>MNE</t>
         </is>
       </c>
       <c r="B1372" t="n">
@@ -37859,14 +37859,14 @@
       </c>
       <c r="F1372" t="inlineStr">
         <is>
-          <t>Türkiye</t>
+          <t>Montenegro</t>
         </is>
       </c>
     </row>
     <row r="1373">
       <c r="A1373" t="inlineStr">
         <is>
-          <t>MNE</t>
+          <t>KWT</t>
         </is>
       </c>
       <c r="B1373" t="n">
@@ -37885,14 +37885,14 @@
       </c>
       <c r="F1373" t="inlineStr">
         <is>
-          <t>Montenegro</t>
+          <t>Kuwait</t>
         </is>
       </c>
     </row>
     <row r="1374">
       <c r="A1374" t="inlineStr">
         <is>
-          <t>KWT</t>
+          <t>BRN</t>
         </is>
       </c>
       <c r="B1374" t="n">
@@ -37911,14 +37911,14 @@
       </c>
       <c r="F1374" t="inlineStr">
         <is>
-          <t>Kuwait</t>
+          <t>Brunei Darussalam</t>
         </is>
       </c>
     </row>
     <row r="1375">
       <c r="A1375" t="inlineStr">
         <is>
-          <t>BRN</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B1375" t="n">
@@ -37937,14 +37937,14 @@
       </c>
       <c r="F1375" t="inlineStr">
         <is>
-          <t>Brunei Darussalam</t>
+          <t>Russia</t>
         </is>
       </c>
     </row>
     <row r="1376">
       <c r="A1376" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>ROU</t>
         </is>
       </c>
       <c r="B1376" t="n">
@@ -37963,14 +37963,14 @@
       </c>
       <c r="F1376" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Romania</t>
         </is>
       </c>
     </row>
     <row r="1377">
       <c r="A1377" t="inlineStr">
         <is>
-          <t>ROU</t>
+          <t>OMN</t>
         </is>
       </c>
       <c r="B1377" t="n">
@@ -37989,14 +37989,14 @@
       </c>
       <c r="F1377" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Oman</t>
         </is>
       </c>
     </row>
     <row r="1378">
       <c r="A1378" t="inlineStr">
         <is>
-          <t>OMN</t>
+          <t>BHS</t>
         </is>
       </c>
       <c r="B1378" t="n">
@@ -38015,14 +38015,14 @@
       </c>
       <c r="F1378" t="inlineStr">
         <is>
-          <t>Oman</t>
+          <t>Bahamas</t>
         </is>
       </c>
     </row>
     <row r="1379">
       <c r="A1379" t="inlineStr">
         <is>
-          <t>BHS</t>
+          <t>KAZ</t>
         </is>
       </c>
       <c r="B1379" t="n">
@@ -38041,14 +38041,14 @@
       </c>
       <c r="F1379" t="inlineStr">
         <is>
-          <t>Bahamas</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
     </row>
     <row r="1380">
       <c r="A1380" t="inlineStr">
         <is>
-          <t>KAZ</t>
+          <t>TTO</t>
         </is>
       </c>
       <c r="B1380" t="n">
@@ -38067,14 +38067,14 @@
       </c>
       <c r="F1380" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
     </row>
     <row r="1381">
       <c r="A1381" t="inlineStr">
         <is>
-          <t>TTO</t>
+          <t>CRI</t>
         </is>
       </c>
       <c r="B1381" t="n">
@@ -38093,14 +38093,14 @@
       </c>
       <c r="F1381" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Costa Rica</t>
         </is>
       </c>
     </row>
     <row r="1382">
       <c r="A1382" t="inlineStr">
         <is>
-          <t>CRI</t>
+          <t>URY</t>
         </is>
       </c>
       <c r="B1382" t="n">
@@ -38119,14 +38119,14 @@
       </c>
       <c r="F1382" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Uruguay</t>
         </is>
       </c>
     </row>
     <row r="1383">
       <c r="A1383" t="inlineStr">
         <is>
-          <t>URY</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="B1383" t="n">
@@ -38145,14 +38145,14 @@
       </c>
       <c r="F1383" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Belarus</t>
         </is>
       </c>
     </row>
     <row r="1384">
       <c r="A1384" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="B1384" t="n">
@@ -38171,14 +38171,14 @@
       </c>
       <c r="F1384" t="inlineStr">
         <is>
-          <t>Belarus</t>
+          <t>Panama</t>
         </is>
       </c>
     </row>
     <row r="1385">
       <c r="A1385" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>MYS</t>
         </is>
       </c>
       <c r="B1385" t="n">
@@ -38197,14 +38197,14 @@
       </c>
       <c r="F1385" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Malaysia</t>
         </is>
       </c>
     </row>
     <row r="1386">
       <c r="A1386" t="inlineStr">
         <is>
-          <t>MYS</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B1386" t="n">
@@ -38223,14 +38223,14 @@
       </c>
       <c r="F1386" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Georgia</t>
         </is>
       </c>
     </row>
     <row r="1387">
       <c r="A1387" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>MUS</t>
         </is>
       </c>
       <c r="B1387" t="n">
@@ -38249,14 +38249,14 @@
       </c>
       <c r="F1387" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Mauritius</t>
         </is>
       </c>
     </row>
     <row r="1388">
       <c r="A1388" t="inlineStr">
         <is>
-          <t>MUS</t>
+          <t>SRB</t>
         </is>
       </c>
       <c r="B1388" t="n">
@@ -38275,14 +38275,14 @@
       </c>
       <c r="F1388" t="inlineStr">
         <is>
-          <t>Mauritius</t>
+          <t>Serbia</t>
         </is>
       </c>
     </row>
     <row r="1389">
       <c r="A1389" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>THA</t>
         </is>
       </c>
       <c r="B1389" t="n">
@@ -38301,14 +38301,14 @@
       </c>
       <c r="F1389" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>Thailand</t>
         </is>
       </c>
     </row>
     <row r="1390">
       <c r="A1390" t="inlineStr">
         <is>
-          <t>THA</t>
+          <t>ALB</t>
         </is>
       </c>
       <c r="B1390" t="n">
@@ -38327,14 +38327,14 @@
       </c>
       <c r="F1390" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>Albania</t>
         </is>
       </c>
     </row>
     <row r="1391">
       <c r="A1391" t="inlineStr">
         <is>
-          <t>ALB</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B1391" t="n">
@@ -38353,14 +38353,14 @@
       </c>
       <c r="F1391" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Bulgaria</t>
         </is>
       </c>
     </row>
     <row r="1392">
       <c r="A1392" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>GRD</t>
         </is>
       </c>
       <c r="B1392" t="n">
@@ -38379,14 +38379,14 @@
       </c>
       <c r="F1392" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Grenada</t>
         </is>
       </c>
     </row>
     <row r="1393">
       <c r="A1393" t="inlineStr">
         <is>
-          <t>GRD</t>
+          <t>BRB</t>
         </is>
       </c>
       <c r="B1393" t="n">
@@ -38405,14 +38405,14 @@
       </c>
       <c r="F1393" t="inlineStr">
         <is>
-          <t>Grenada</t>
+          <t>Barbados</t>
         </is>
       </c>
     </row>
     <row r="1394">
       <c r="A1394" t="inlineStr">
         <is>
-          <t>BRB</t>
+          <t>ATG</t>
         </is>
       </c>
       <c r="B1394" t="n">
@@ -38431,14 +38431,14 @@
       </c>
       <c r="F1394" t="inlineStr">
         <is>
-          <t>Barbados</t>
+          <t>Antigua and Barbuda</t>
         </is>
       </c>
     </row>
     <row r="1395">
       <c r="A1395" t="inlineStr">
         <is>
-          <t>ATG</t>
+          <t>SYC</t>
         </is>
       </c>
       <c r="B1395" t="n">
@@ -38457,14 +38457,14 @@
       </c>
       <c r="F1395" t="inlineStr">
         <is>
-          <t>Antigua and Barbuda</t>
+          <t>Seychelles</t>
         </is>
       </c>
     </row>
     <row r="1396">
       <c r="A1396" t="inlineStr">
         <is>
-          <t>SYC</t>
+          <t>LKA</t>
         </is>
       </c>
       <c r="B1396" t="n">
@@ -38483,14 +38483,14 @@
       </c>
       <c r="F1396" t="inlineStr">
         <is>
-          <t>Seychelles</t>
+          <t>Sri Lanka</t>
         </is>
       </c>
     </row>
     <row r="1397">
       <c r="A1397" t="inlineStr">
         <is>
-          <t>LKA</t>
+          <t>BIH</t>
         </is>
       </c>
       <c r="B1397" t="n">
@@ -38509,14 +38509,14 @@
       </c>
       <c r="F1397" t="inlineStr">
         <is>
-          <t>Sri Lanka</t>
+          <t>Bosnia and Herzegovina</t>
         </is>
       </c>
     </row>
     <row r="1398">
       <c r="A1398" t="inlineStr">
         <is>
-          <t>BIH</t>
+          <t>KNA</t>
         </is>
       </c>
       <c r="B1398" t="n">
@@ -38535,14 +38535,14 @@
       </c>
       <c r="F1398" t="inlineStr">
         <is>
-          <t>Bosnia and Herzegovina</t>
+          <t>St. Kitts and Nevis</t>
         </is>
       </c>
     </row>
     <row r="1399">
       <c r="A1399" t="inlineStr">
         <is>
-          <t>KNA</t>
+          <t>IRN</t>
         </is>
       </c>
       <c r="B1399" t="n">
@@ -38561,14 +38561,14 @@
       </c>
       <c r="F1399" t="inlineStr">
         <is>
-          <t>St. Kitts and Nevis</t>
+          <t>Iran</t>
         </is>
       </c>
     </row>
     <row r="1400">
       <c r="A1400" t="inlineStr">
         <is>
-          <t>IRN</t>
+          <t>UKR</t>
         </is>
       </c>
       <c r="B1400" t="n">
@@ -38587,14 +38587,14 @@
       </c>
       <c r="F1400" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Ukraine</t>
         </is>
       </c>
     </row>
     <row r="1401">
       <c r="A1401" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>MKD</t>
         </is>
       </c>
       <c r="B1401" t="n">
@@ -38613,14 +38613,14 @@
       </c>
       <c r="F1401" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>North Macedonia</t>
         </is>
       </c>
     </row>
     <row r="1402">
       <c r="A1402" t="inlineStr">
         <is>
-          <t>MKD</t>
+          <t>CHN</t>
         </is>
       </c>
       <c r="B1402" t="n">
@@ -38639,14 +38639,14 @@
       </c>
       <c r="F1402" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>China</t>
         </is>
       </c>
     </row>
     <row r="1403">
       <c r="A1403" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>DOM</t>
         </is>
       </c>
       <c r="B1403" t="n">
@@ -38665,14 +38665,14 @@
       </c>
       <c r="F1403" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
     </row>
     <row r="1404">
       <c r="A1404" t="inlineStr">
         <is>
-          <t>DOM</t>
+          <t>MDA</t>
         </is>
       </c>
       <c r="B1404" t="n">
@@ -38691,14 +38691,14 @@
       </c>
       <c r="F1404" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Moldova</t>
         </is>
       </c>
     </row>
     <row r="1405">
       <c r="A1405" t="inlineStr">
         <is>
-          <t>MDA</t>
+          <t>PLW</t>
         </is>
       </c>
       <c r="B1405" t="n">
@@ -38717,14 +38717,14 @@
       </c>
       <c r="F1405" t="inlineStr">
         <is>
-          <t>Moldova</t>
+          <t>Palau</t>
         </is>
       </c>
     </row>
     <row r="1406">
       <c r="A1406" t="inlineStr">
         <is>
-          <t>PLW</t>
+          <t>CUB</t>
         </is>
       </c>
       <c r="B1406" t="n">
@@ -38743,14 +38743,14 @@
       </c>
       <c r="F1406" t="inlineStr">
         <is>
-          <t>Palau</t>
+          <t>Cuba</t>
         </is>
       </c>
     </row>
     <row r="1407">
       <c r="A1407" t="inlineStr">
         <is>
-          <t>CUB</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B1407" t="n">
@@ -38769,14 +38769,14 @@
       </c>
       <c r="F1407" t="inlineStr">
         <is>
-          <t>Cuba</t>
+          <t>Peru</t>
         </is>
       </c>
     </row>
     <row r="1408">
       <c r="A1408" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>ARM</t>
         </is>
       </c>
       <c r="B1408" t="n">
@@ -38795,14 +38795,14 @@
       </c>
       <c r="F1408" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Armenia</t>
         </is>
       </c>
     </row>
     <row r="1409">
       <c r="A1409" t="inlineStr">
         <is>
-          <t>ARM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B1409" t="n">
@@ -38821,14 +38821,14 @@
       </c>
       <c r="F1409" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Mexico</t>
         </is>
       </c>
     </row>
     <row r="1410">
       <c r="A1410" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>BRA</t>
         </is>
       </c>
       <c r="B1410" t="n">
@@ -38847,14 +38847,14 @@
       </c>
       <c r="F1410" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Brazil</t>
         </is>
       </c>
     </row>
     <row r="1411">
       <c r="A1411" t="inlineStr">
         <is>
-          <t>BRA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="B1411" t="n">
@@ -38873,14 +38873,14 @@
       </c>
       <c r="F1411" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Colombia</t>
         </is>
       </c>
     </row>
     <row r="1412">
       <c r="A1412" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>VCT</t>
         </is>
       </c>
       <c r="B1412" t="n">
@@ -38899,14 +38899,14 @@
       </c>
       <c r="F1412" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>St. Vincent and the Grenadines</t>
         </is>
       </c>
     </row>
     <row r="1413">
       <c r="A1413" t="inlineStr">
         <is>
-          <t>VCT</t>
+          <t>MDV</t>
         </is>
       </c>
       <c r="B1413" t="n">
@@ -38925,14 +38925,14 @@
       </c>
       <c r="F1413" t="inlineStr">
         <is>
-          <t>St. Vincent and the Grenadines</t>
+          <t>Maldives</t>
         </is>
       </c>
     </row>
     <row r="1414">
       <c r="A1414" t="inlineStr">
         <is>
-          <t>MDV</t>
+          <t>DZA</t>
         </is>
       </c>
       <c r="B1414" t="n">
@@ -38951,14 +38951,14 @@
       </c>
       <c r="F1414" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Algeria</t>
         </is>
       </c>
     </row>
     <row r="1415">
       <c r="A1415" t="inlineStr">
         <is>
-          <t>DZA</t>
+          <t>AZE</t>
         </is>
       </c>
       <c r="B1415" t="n">
@@ -38977,14 +38977,14 @@
       </c>
       <c r="F1415" t="inlineStr">
         <is>
-          <t>Algeria</t>
+          <t>Azerbaijan</t>
         </is>
       </c>
     </row>
     <row r="1416">
       <c r="A1416" t="inlineStr">
         <is>
-          <t>AZE</t>
+          <t>TON</t>
         </is>
       </c>
       <c r="B1416" t="n">
@@ -39003,14 +39003,14 @@
       </c>
       <c r="F1416" t="inlineStr">
         <is>
-          <t>Azerbaijan</t>
+          <t>Tonga</t>
         </is>
       </c>
     </row>
     <row r="1417">
       <c r="A1417" t="inlineStr">
         <is>
-          <t>TON</t>
+          <t>TKM</t>
         </is>
       </c>
       <c r="B1417" t="n">
@@ -39029,14 +39029,14 @@
       </c>
       <c r="F1417" t="inlineStr">
         <is>
-          <t>Tonga</t>
+          <t>Turkmenistan</t>
         </is>
       </c>
     </row>
     <row r="1418">
       <c r="A1418" t="inlineStr">
         <is>
-          <t>TKM</t>
+          <t>ECU</t>
         </is>
       </c>
       <c r="B1418" t="n">
@@ -39055,14 +39055,14 @@
       </c>
       <c r="F1418" t="inlineStr">
         <is>
-          <t>Turkmenistan</t>
+          <t>Ecuador</t>
         </is>
       </c>
     </row>
     <row r="1419">
       <c r="A1419" t="inlineStr">
         <is>
-          <t>ECU</t>
+          <t>MNG</t>
         </is>
       </c>
       <c r="B1419" t="n">
@@ -39081,14 +39081,14 @@
       </c>
       <c r="F1419" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Mongolia</t>
         </is>
       </c>
     </row>
     <row r="1420">
       <c r="A1420" t="inlineStr">
         <is>
-          <t>MNG</t>
+          <t>EGY</t>
         </is>
       </c>
       <c r="B1420" t="n">
@@ -39107,14 +39107,14 @@
       </c>
       <c r="F1420" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Egypt</t>
         </is>
       </c>
     </row>
     <row r="1421">
       <c r="A1421" t="inlineStr">
         <is>
-          <t>EGY</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="B1421" t="n">
@@ -39133,14 +39133,14 @@
       </c>
       <c r="F1421" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Tunisia</t>
         </is>
       </c>
     </row>
     <row r="1422">
       <c r="A1422" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>FJI</t>
         </is>
       </c>
       <c r="B1422" t="n">
@@ -39159,14 +39159,14 @@
       </c>
       <c r="F1422" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>Fiji</t>
         </is>
       </c>
     </row>
     <row r="1423">
       <c r="A1423" t="inlineStr">
         <is>
-          <t>FJI</t>
+          <t>SUR</t>
         </is>
       </c>
       <c r="B1423" t="n">
@@ -39185,14 +39185,14 @@
       </c>
       <c r="F1423" t="inlineStr">
         <is>
-          <t>Fiji</t>
+          <t>Suriname</t>
         </is>
       </c>
     </row>
     <row r="1424">
       <c r="A1424" t="inlineStr">
         <is>
-          <t>SUR</t>
+          <t>UZB</t>
         </is>
       </c>
       <c r="B1424" t="n">
@@ -39211,14 +39211,14 @@
       </c>
       <c r="F1424" t="inlineStr">
         <is>
-          <t>Suriname</t>
+          <t>Uzbekistan</t>
         </is>
       </c>
     </row>
     <row r="1425">
       <c r="A1425" t="inlineStr">
         <is>
-          <t>UZB</t>
+          <t>DMA</t>
         </is>
       </c>
       <c r="B1425" t="n">
@@ -39237,14 +39237,14 @@
       </c>
       <c r="F1425" t="inlineStr">
         <is>
-          <t>Uzbekistan</t>
+          <t>Dominica</t>
         </is>
       </c>
     </row>
     <row r="1426">
       <c r="A1426" t="inlineStr">
         <is>
-          <t>DMA</t>
+          <t>JOR</t>
         </is>
       </c>
       <c r="B1426" t="n">
@@ -39263,14 +39263,14 @@
       </c>
       <c r="F1426" t="inlineStr">
         <is>
-          <t>Dominica</t>
+          <t>Jordan</t>
         </is>
       </c>
     </row>
     <row r="1427">
       <c r="A1427" t="inlineStr">
         <is>
-          <t>JOR</t>
+          <t>LBY</t>
         </is>
       </c>
       <c r="B1427" t="n">
@@ -39289,14 +39289,14 @@
       </c>
       <c r="F1427" t="inlineStr">
         <is>
-          <t>Jordan</t>
+          <t>Libya</t>
         </is>
       </c>
     </row>
     <row r="1428">
       <c r="A1428" t="inlineStr">
         <is>
-          <t>LBY</t>
+          <t>PRY</t>
         </is>
       </c>
       <c r="B1428" t="n">
@@ -39315,14 +39315,14 @@
       </c>
       <c r="F1428" t="inlineStr">
         <is>
-          <t>Libya</t>
+          <t>Paraguay</t>
         </is>
       </c>
     </row>
     <row r="1429">
       <c r="A1429" t="inlineStr">
         <is>
-          <t>PRY</t>
+          <t>PSE</t>
         </is>
       </c>
       <c r="B1429" t="n">
@@ -39341,14 +39341,14 @@
       </c>
       <c r="F1429" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Palestine</t>
         </is>
       </c>
     </row>
     <row r="1430">
       <c r="A1430" t="inlineStr">
         <is>
-          <t>PSE</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B1430" t="n">
@@ -39367,14 +39367,14 @@
       </c>
       <c r="F1430" t="inlineStr">
         <is>
-          <t>Palestine</t>
+          <t>St. Lucia</t>
         </is>
       </c>
     </row>
     <row r="1431">
       <c r="A1431" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>GUY</t>
         </is>
       </c>
       <c r="B1431" t="n">
@@ -39393,14 +39393,14 @@
       </c>
       <c r="F1431" t="inlineStr">
         <is>
-          <t>St. Lucia</t>
+          <t>Guyana</t>
         </is>
       </c>
     </row>
     <row r="1432">
       <c r="A1432" t="inlineStr">
         <is>
-          <t>GUY</t>
+          <t>ZAF</t>
         </is>
       </c>
       <c r="B1432" t="n">
@@ -39419,14 +39419,14 @@
       </c>
       <c r="F1432" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>South Africa</t>
         </is>
       </c>
     </row>
     <row r="1433">
       <c r="A1433" t="inlineStr">
         <is>
-          <t>ZAF</t>
+          <t>JAM</t>
         </is>
       </c>
       <c r="B1433" t="n">
@@ -39445,14 +39445,14 @@
       </c>
       <c r="F1433" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Jamaica</t>
         </is>
       </c>
     </row>
     <row r="1434">
       <c r="A1434" t="inlineStr">
         <is>
-          <t>JAM</t>
+          <t>WSM</t>
         </is>
       </c>
       <c r="B1434" t="n">
@@ -39471,14 +39471,14 @@
       </c>
       <c r="F1434" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>Samoa</t>
         </is>
       </c>
     </row>
     <row r="1435">
       <c r="A1435" t="inlineStr">
         <is>
-          <t>WSM</t>
+          <t>GAB</t>
         </is>
       </c>
       <c r="B1435" t="n">
@@ -39497,14 +39497,14 @@
       </c>
       <c r="F1435" t="inlineStr">
         <is>
-          <t>Samoa</t>
+          <t>Gabon</t>
         </is>
       </c>
     </row>
     <row r="1436">
       <c r="A1436" t="inlineStr">
         <is>
-          <t>GAB</t>
+          <t>LBN</t>
         </is>
       </c>
       <c r="B1436" t="n">
@@ -39523,14 +39523,14 @@
       </c>
       <c r="F1436" t="inlineStr">
         <is>
-          <t>Gabon</t>
+          <t>Lebanon</t>
         </is>
       </c>
     </row>
     <row r="1437">
       <c r="A1437" t="inlineStr">
         <is>
-          <t>LBN</t>
+          <t>IDN</t>
         </is>
       </c>
       <c r="B1437" t="n">
@@ -39549,14 +39549,14 @@
       </c>
       <c r="F1437" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Indonesia</t>
         </is>
       </c>
     </row>
     <row r="1438">
       <c r="A1438" t="inlineStr">
         <is>
-          <t>IDN</t>
+          <t>VNM</t>
         </is>
       </c>
       <c r="B1438" t="n">
@@ -39575,14 +39575,14 @@
       </c>
       <c r="F1438" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Vietnam</t>
         </is>
       </c>
     </row>
     <row r="1439">
       <c r="A1439" t="inlineStr">
         <is>
-          <t>VNM</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B1439" t="n">
@@ -39601,14 +39601,14 @@
       </c>
       <c r="F1439" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Philippines</t>
         </is>
       </c>
     </row>
     <row r="1440">
       <c r="A1440" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>BWA</t>
         </is>
       </c>
       <c r="B1440" t="n">
@@ -39627,14 +39627,14 @@
       </c>
       <c r="F1440" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Botswana</t>
         </is>
       </c>
     </row>
     <row r="1441">
       <c r="A1441" t="inlineStr">
         <is>
-          <t>BWA</t>
+          <t>BOL</t>
         </is>
       </c>
       <c r="B1441" t="n">
@@ -39653,14 +39653,14 @@
       </c>
       <c r="F1441" t="inlineStr">
         <is>
-          <t>Botswana</t>
+          <t>Bolivia</t>
         </is>
       </c>
     </row>
     <row r="1442">
       <c r="A1442" t="inlineStr">
         <is>
-          <t>BOL</t>
+          <t>KGZ</t>
         </is>
       </c>
       <c r="B1442" t="n">
@@ -39679,14 +39679,14 @@
       </c>
       <c r="F1442" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Kyrgyz Republic</t>
         </is>
       </c>
     </row>
     <row r="1443">
       <c r="A1443" t="inlineStr">
         <is>
-          <t>KGZ</t>
+          <t>VEN</t>
         </is>
       </c>
       <c r="B1443" t="n">
@@ -39705,14 +39705,14 @@
       </c>
       <c r="F1443" t="inlineStr">
         <is>
-          <t>Kyrgyz Republic</t>
+          <t>Venezuela</t>
         </is>
       </c>
     </row>
     <row r="1444">
       <c r="A1444" t="inlineStr">
         <is>
-          <t>VEN</t>
+          <t>IRQ</t>
         </is>
       </c>
       <c r="B1444" t="n">
@@ -39731,14 +39731,14 @@
       </c>
       <c r="F1444" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>Iraq</t>
         </is>
       </c>
     </row>
     <row r="1445">
       <c r="A1445" t="inlineStr">
         <is>
-          <t>IRQ</t>
+          <t>TJK</t>
         </is>
       </c>
       <c r="B1445" t="n">
@@ -39757,14 +39757,14 @@
       </c>
       <c r="F1445" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Tajikistan</t>
         </is>
       </c>
     </row>
     <row r="1446">
       <c r="A1446" t="inlineStr">
         <is>
-          <t>TJK</t>
+          <t>BLZ</t>
         </is>
       </c>
       <c r="B1446" t="n">
@@ -39783,14 +39783,14 @@
       </c>
       <c r="F1446" t="inlineStr">
         <is>
-          <t>Tajikistan</t>
+          <t>Belize</t>
         </is>
       </c>
     </row>
     <row r="1447">
       <c r="A1447" t="inlineStr">
         <is>
-          <t>BLZ</t>
+          <t>MAR</t>
         </is>
       </c>
       <c r="B1447" t="n">
@@ -39809,14 +39809,14 @@
       </c>
       <c r="F1447" t="inlineStr">
         <is>
-          <t>Belize</t>
+          <t>Morocco</t>
         </is>
       </c>
     </row>
     <row r="1448">
       <c r="A1448" t="inlineStr">
         <is>
-          <t>MAR</t>
+          <t>SLV</t>
         </is>
       </c>
       <c r="B1448" t="n">
@@ -39835,14 +39835,14 @@
       </c>
       <c r="F1448" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>El Salvador</t>
         </is>
       </c>
     </row>
     <row r="1449">
       <c r="A1449" t="inlineStr">
         <is>
-          <t>SLV</t>
+          <t>NIC</t>
         </is>
       </c>
       <c r="B1449" t="n">
@@ -39861,14 +39861,14 @@
       </c>
       <c r="F1449" t="inlineStr">
         <is>
-          <t>El Salvador</t>
+          <t>Nicaragua</t>
         </is>
       </c>
     </row>
     <row r="1450">
       <c r="A1450" t="inlineStr">
         <is>
-          <t>NIC</t>
+          <t>BTN</t>
         </is>
       </c>
       <c r="B1450" t="n">
@@ -39887,14 +39887,14 @@
       </c>
       <c r="F1450" t="inlineStr">
         <is>
-          <t>Nicaragua</t>
+          <t>Bhutan</t>
         </is>
       </c>
     </row>
     <row r="1451">
       <c r="A1451" t="inlineStr">
         <is>
-          <t>BTN</t>
+          <t>CPV</t>
         </is>
       </c>
       <c r="B1451" t="n">
@@ -39913,14 +39913,14 @@
       </c>
       <c r="F1451" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>Cabo Verde</t>
         </is>
       </c>
     </row>
     <row r="1452">
       <c r="A1452" t="inlineStr">
         <is>
-          <t>CPV</t>
+          <t>BGD</t>
         </is>
       </c>
       <c r="B1452" t="n">
@@ -39939,14 +39939,14 @@
       </c>
       <c r="F1452" t="inlineStr">
         <is>
-          <t>Cabo Verde</t>
+          <t>Bangladesh</t>
         </is>
       </c>
     </row>
     <row r="1453">
       <c r="A1453" t="inlineStr">
         <is>
-          <t>BGD</t>
+          <t>TUV</t>
         </is>
       </c>
       <c r="B1453" t="n">
@@ -39965,14 +39965,14 @@
       </c>
       <c r="F1453" t="inlineStr">
         <is>
-          <t>Bangladesh</t>
+          <t>Tuvalu</t>
         </is>
       </c>
     </row>
     <row r="1454">
       <c r="A1454" t="inlineStr">
         <is>
-          <t>TUV</t>
+          <t>MHL</t>
         </is>
       </c>
       <c r="B1454" t="n">
@@ -39991,14 +39991,14 @@
       </c>
       <c r="F1454" t="inlineStr">
         <is>
-          <t>Tuvalu</t>
+          <t>Marshall Islands</t>
         </is>
       </c>
     </row>
     <row r="1455">
       <c r="A1455" t="inlineStr">
         <is>
-          <t>MHL</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B1455" t="n">
@@ -40017,14 +40017,14 @@
       </c>
       <c r="F1455" t="inlineStr">
         <is>
-          <t>Marshall Islands</t>
+          <t>India</t>
         </is>
       </c>
     </row>
     <row r="1456">
       <c r="A1456" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>GHA</t>
         </is>
       </c>
       <c r="B1456" t="n">
@@ -40043,14 +40043,14 @@
       </c>
       <c r="F1456" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Ghana</t>
         </is>
       </c>
     </row>
     <row r="1457">
       <c r="A1457" t="inlineStr">
         <is>
-          <t>GHA</t>
+          <t>FSM</t>
         </is>
       </c>
       <c r="B1457" t="n">
@@ -40069,14 +40069,14 @@
       </c>
       <c r="F1457" t="inlineStr">
         <is>
-          <t>Ghana</t>
+          <t>Micronesia, Fed. Sts.</t>
         </is>
       </c>
     </row>
     <row r="1458">
       <c r="A1458" t="inlineStr">
         <is>
-          <t>FSM</t>
+          <t>GTM</t>
         </is>
       </c>
       <c r="B1458" t="n">
@@ -40095,14 +40095,14 @@
       </c>
       <c r="F1458" t="inlineStr">
         <is>
-          <t>Micronesia, Fed. Sts.</t>
+          <t>Guatemala</t>
         </is>
       </c>
     </row>
     <row r="1459">
       <c r="A1459" t="inlineStr">
         <is>
-          <t>GTM</t>
+          <t>KIR</t>
         </is>
       </c>
       <c r="B1459" t="n">
@@ -40121,14 +40121,14 @@
       </c>
       <c r="F1459" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Kiribati</t>
         </is>
       </c>
     </row>
     <row r="1460">
       <c r="A1460" t="inlineStr">
         <is>
-          <t>KIR</t>
+          <t>HND</t>
         </is>
       </c>
       <c r="B1460" t="n">
@@ -40147,14 +40147,14 @@
       </c>
       <c r="F1460" t="inlineStr">
         <is>
-          <t>Kiribati</t>
+          <t>Honduras</t>
         </is>
       </c>
     </row>
     <row r="1461">
       <c r="A1461" t="inlineStr">
         <is>
-          <t>HND</t>
+          <t>STP</t>
         </is>
       </c>
       <c r="B1461" t="n">
@@ -40173,14 +40173,14 @@
       </c>
       <c r="F1461" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Sao Tome and Principe</t>
         </is>
       </c>
     </row>
     <row r="1462">
       <c r="A1462" t="inlineStr">
         <is>
-          <t>STP</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="B1462" t="n">
@@ -40199,14 +40199,14 @@
       </c>
       <c r="F1462" t="inlineStr">
         <is>
-          <t>Sao Tome and Principe</t>
+          <t>Namibia</t>
         </is>
       </c>
     </row>
     <row r="1463">
       <c r="A1463" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>LAO</t>
         </is>
       </c>
       <c r="B1463" t="n">
@@ -40225,14 +40225,14 @@
       </c>
       <c r="F1463" t="inlineStr">
         <is>
-          <t>Namibia</t>
+          <t>Laos</t>
         </is>
       </c>
     </row>
     <row r="1464">
       <c r="A1464" t="inlineStr">
         <is>
-          <t>LAO</t>
+          <t>TLS</t>
         </is>
       </c>
       <c r="B1464" t="n">
@@ -40251,14 +40251,14 @@
       </c>
       <c r="F1464" t="inlineStr">
         <is>
-          <t>Laos</t>
+          <t>Timor-Leste</t>
         </is>
       </c>
     </row>
     <row r="1465">
       <c r="A1465" t="inlineStr">
         <is>
-          <t>TLS</t>
+          <t>VUT</t>
         </is>
       </c>
       <c r="B1465" t="n">
@@ -40277,14 +40277,14 @@
       </c>
       <c r="F1465" t="inlineStr">
         <is>
-          <t>Timor-Leste</t>
+          <t>Vanuatu</t>
         </is>
       </c>
     </row>
     <row r="1466">
       <c r="A1466" t="inlineStr">
         <is>
-          <t>VUT</t>
+          <t>NPL</t>
         </is>
       </c>
       <c r="B1466" t="n">
@@ -40303,14 +40303,14 @@
       </c>
       <c r="F1466" t="inlineStr">
         <is>
-          <t>Vanuatu</t>
+          <t>Nepal</t>
         </is>
       </c>
     </row>
     <row r="1467">
       <c r="A1467" t="inlineStr">
         <is>
-          <t>NPL</t>
+          <t>SWZ</t>
         </is>
       </c>
       <c r="B1467" t="n">
@@ -40329,14 +40329,14 @@
       </c>
       <c r="F1467" t="inlineStr">
         <is>
-          <t>Nepal</t>
+          <t>Eswatini</t>
         </is>
       </c>
     </row>
     <row r="1468">
       <c r="A1468" t="inlineStr">
         <is>
-          <t>SWZ</t>
+          <t>GNQ</t>
         </is>
       </c>
       <c r="B1468" t="n">
@@ -40355,14 +40355,14 @@
       </c>
       <c r="F1468" t="inlineStr">
         <is>
-          <t>Eswatini</t>
+          <t>Equatorial Guinea</t>
         </is>
       </c>
     </row>
     <row r="1469">
       <c r="A1469" t="inlineStr">
         <is>
-          <t>GNQ</t>
+          <t>KHM</t>
         </is>
       </c>
       <c r="B1469" t="n">
@@ -40381,14 +40381,14 @@
       </c>
       <c r="F1469" t="inlineStr">
         <is>
-          <t>Equatorial Guinea</t>
+          <t>Cambodia</t>
         </is>
       </c>
     </row>
     <row r="1470">
       <c r="A1470" t="inlineStr">
         <is>
-          <t>KHM</t>
+          <t>ZWE</t>
         </is>
       </c>
       <c r="B1470" t="n">
@@ -40407,14 +40407,14 @@
       </c>
       <c r="F1470" t="inlineStr">
         <is>
-          <t>Cambodia</t>
+          <t>Zimbabwe</t>
         </is>
       </c>
     </row>
     <row r="1471">
       <c r="A1471" t="inlineStr">
         <is>
-          <t>ZWE</t>
+          <t>AGO</t>
         </is>
       </c>
       <c r="B1471" t="n">
@@ -40433,14 +40433,14 @@
       </c>
       <c r="F1471" t="inlineStr">
         <is>
-          <t>Zimbabwe</t>
+          <t>Angola</t>
         </is>
       </c>
     </row>
     <row r="1472">
       <c r="A1472" t="inlineStr">
         <is>
-          <t>AGO</t>
+          <t>MMR</t>
         </is>
       </c>
       <c r="B1472" t="n">
@@ -40459,14 +40459,14 @@
       </c>
       <c r="F1472" t="inlineStr">
         <is>
-          <t>Angola</t>
+          <t>Myanmar</t>
         </is>
       </c>
     </row>
     <row r="1473">
       <c r="A1473" t="inlineStr">
         <is>
-          <t>MMR</t>
+          <t>SYR</t>
         </is>
       </c>
       <c r="B1473" t="n">
@@ -40485,14 +40485,14 @@
       </c>
       <c r="F1473" t="inlineStr">
         <is>
-          <t>Myanmar</t>
+          <t>Syria</t>
         </is>
       </c>
     </row>
     <row r="1474">
       <c r="A1474" t="inlineStr">
         <is>
-          <t>SYR</t>
+          <t>CMR</t>
         </is>
       </c>
       <c r="B1474" t="n">
@@ -40511,14 +40511,14 @@
       </c>
       <c r="F1474" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Cameroon</t>
         </is>
       </c>
     </row>
     <row r="1475">
       <c r="A1475" t="inlineStr">
         <is>
-          <t>CMR</t>
+          <t>KEN</t>
         </is>
       </c>
       <c r="B1475" t="n">
@@ -40537,14 +40537,14 @@
       </c>
       <c r="F1475" t="inlineStr">
         <is>
-          <t>Cameroon</t>
+          <t>Kenya</t>
         </is>
       </c>
     </row>
     <row r="1476">
       <c r="A1476" t="inlineStr">
         <is>
-          <t>KEN</t>
+          <t>COG</t>
         </is>
       </c>
       <c r="B1476" t="n">
@@ -40563,14 +40563,14 @@
       </c>
       <c r="F1476" t="inlineStr">
         <is>
-          <t>Kenya</t>
+          <t>Congo Republic</t>
         </is>
       </c>
     </row>
     <row r="1477">
       <c r="A1477" t="inlineStr">
         <is>
-          <t>COG</t>
+          <t>ZMB</t>
         </is>
       </c>
       <c r="B1477" t="n">
@@ -40589,14 +40589,14 @@
       </c>
       <c r="F1477" t="inlineStr">
         <is>
-          <t>Congo Republic</t>
+          <t>Zambia</t>
         </is>
       </c>
     </row>
     <row r="1478">
       <c r="A1478" t="inlineStr">
         <is>
-          <t>ZMB</t>
+          <t>SLB</t>
         </is>
       </c>
       <c r="B1478" t="n">
@@ -40615,14 +40615,14 @@
       </c>
       <c r="F1478" t="inlineStr">
         <is>
-          <t>Zambia</t>
+          <t>Solomon Islands</t>
         </is>
       </c>
     </row>
     <row r="1479">
       <c r="A1479" t="inlineStr">
         <is>
-          <t>SLB</t>
+          <t>COM</t>
         </is>
       </c>
       <c r="B1479" t="n">
@@ -40641,14 +40641,14 @@
       </c>
       <c r="F1479" t="inlineStr">
         <is>
-          <t>Solomon Islands</t>
+          <t>Comoros</t>
         </is>
       </c>
     </row>
     <row r="1480">
       <c r="A1480" t="inlineStr">
         <is>
-          <t>COM</t>
+          <t>PNG</t>
         </is>
       </c>
       <c r="B1480" t="n">
@@ -40667,14 +40667,14 @@
       </c>
       <c r="F1480" t="inlineStr">
         <is>
-          <t>Comoros</t>
+          <t>Papua New Guinea</t>
         </is>
       </c>
     </row>
     <row r="1481">
       <c r="A1481" t="inlineStr">
         <is>
-          <t>PNG</t>
+          <t>MRT</t>
         </is>
       </c>
       <c r="B1481" t="n">
@@ -40693,14 +40693,14 @@
       </c>
       <c r="F1481" t="inlineStr">
         <is>
-          <t>Papua New Guinea</t>
+          <t>Mauritania</t>
         </is>
       </c>
     </row>
     <row r="1482">
       <c r="A1482" t="inlineStr">
         <is>
-          <t>MRT</t>
+          <t>CIV</t>
         </is>
       </c>
       <c r="B1482" t="n">
@@ -40719,14 +40719,14 @@
       </c>
       <c r="F1482" t="inlineStr">
         <is>
-          <t>Mauritania</t>
+          <t>Cote d'Ivoire</t>
         </is>
       </c>
     </row>
     <row r="1483">
       <c r="A1483" t="inlineStr">
         <is>
-          <t>CIV</t>
+          <t>TZA</t>
         </is>
       </c>
       <c r="B1483" t="n">
@@ -40745,14 +40745,14 @@
       </c>
       <c r="F1483" t="inlineStr">
         <is>
-          <t>Cote d'Ivoire</t>
+          <t>Tanzania</t>
         </is>
       </c>
     </row>
     <row r="1484">
       <c r="A1484" t="inlineStr">
         <is>
-          <t>TZA</t>
+          <t>PAK</t>
         </is>
       </c>
       <c r="B1484" t="n">
@@ -40771,14 +40771,14 @@
       </c>
       <c r="F1484" t="inlineStr">
         <is>
-          <t>Tanzania</t>
+          <t>Pakistan</t>
         </is>
       </c>
     </row>
     <row r="1485">
       <c r="A1485" t="inlineStr">
         <is>
-          <t>PAK</t>
+          <t>TGO</t>
         </is>
       </c>
       <c r="B1485" t="n">
@@ -40797,14 +40797,14 @@
       </c>
       <c r="F1485" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Togo</t>
         </is>
       </c>
     </row>
     <row r="1486">
       <c r="A1486" t="inlineStr">
         <is>
-          <t>TGO</t>
+          <t>HTI</t>
         </is>
       </c>
       <c r="B1486" t="n">
@@ -40823,14 +40823,14 @@
       </c>
       <c r="F1486" t="inlineStr">
         <is>
-          <t>Togo</t>
+          <t>Haiti</t>
         </is>
       </c>
     </row>
     <row r="1487">
       <c r="A1487" t="inlineStr">
         <is>
-          <t>HTI</t>
+          <t>NGA</t>
         </is>
       </c>
       <c r="B1487" t="n">
@@ -40849,14 +40849,14 @@
       </c>
       <c r="F1487" t="inlineStr">
         <is>
-          <t>Haiti</t>
+          <t>Nigeria</t>
         </is>
       </c>
     </row>
     <row r="1488">
       <c r="A1488" t="inlineStr">
         <is>
-          <t>NGA</t>
+          <t>RWA</t>
         </is>
       </c>
       <c r="B1488" t="n">
@@ -40875,14 +40875,14 @@
       </c>
       <c r="F1488" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Rwanda</t>
         </is>
       </c>
     </row>
     <row r="1489">
       <c r="A1489" t="inlineStr">
         <is>
-          <t>RWA</t>
+          <t>BEN</t>
         </is>
       </c>
       <c r="B1489" t="n">
@@ -40901,14 +40901,14 @@
       </c>
       <c r="F1489" t="inlineStr">
         <is>
-          <t>Rwanda</t>
+          <t>Benin</t>
         </is>
       </c>
     </row>
     <row r="1490">
       <c r="A1490" t="inlineStr">
         <is>
-          <t>BEN</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="B1490" t="n">
@@ -40927,14 +40927,14 @@
       </c>
       <c r="F1490" t="inlineStr">
         <is>
-          <t>Benin</t>
+          <t>Uganda</t>
         </is>
       </c>
     </row>
     <row r="1491">
       <c r="A1491" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>LSO</t>
         </is>
       </c>
       <c r="B1491" t="n">
@@ -40953,14 +40953,14 @@
       </c>
       <c r="F1491" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Lesotho</t>
         </is>
       </c>
     </row>
     <row r="1492">
       <c r="A1492" t="inlineStr">
         <is>
-          <t>LSO</t>
+          <t>MWI</t>
         </is>
       </c>
       <c r="B1492" t="n">
@@ -40979,14 +40979,14 @@
       </c>
       <c r="F1492" t="inlineStr">
         <is>
-          <t>Lesotho</t>
+          <t>Malawi</t>
         </is>
       </c>
     </row>
     <row r="1493">
       <c r="A1493" t="inlineStr">
         <is>
-          <t>MWI</t>
+          <t>SEN</t>
         </is>
       </c>
       <c r="B1493" t="n">
@@ -41005,14 +41005,14 @@
       </c>
       <c r="F1493" t="inlineStr">
         <is>
-          <t>Malawi</t>
+          <t>Senegal</t>
         </is>
       </c>
     </row>
     <row r="1494">
       <c r="A1494" t="inlineStr">
         <is>
-          <t>SEN</t>
+          <t>DJI</t>
         </is>
       </c>
       <c r="B1494" t="n">
@@ -41031,14 +41031,14 @@
       </c>
       <c r="F1494" t="inlineStr">
         <is>
-          <t>Senegal</t>
+          <t>Djibouti</t>
         </is>
       </c>
     </row>
     <row r="1495">
       <c r="A1495" t="inlineStr">
         <is>
-          <t>DJI</t>
+          <t>SDN</t>
         </is>
       </c>
       <c r="B1495" t="n">
@@ -41057,14 +41057,14 @@
       </c>
       <c r="F1495" t="inlineStr">
         <is>
-          <t>Djibouti</t>
+          <t>Sudan</t>
         </is>
       </c>
     </row>
     <row r="1496">
       <c r="A1496" t="inlineStr">
         <is>
-          <t>SDN</t>
+          <t>MDG</t>
         </is>
       </c>
       <c r="B1496" t="n">
@@ -41083,14 +41083,14 @@
       </c>
       <c r="F1496" t="inlineStr">
         <is>
-          <t>Sudan</t>
+          <t>Madagascar</t>
         </is>
       </c>
     </row>
     <row r="1497">
       <c r="A1497" t="inlineStr">
         <is>
-          <t>MDG</t>
+          <t>GMB</t>
         </is>
       </c>
       <c r="B1497" t="n">
@@ -41109,14 +41109,14 @@
       </c>
       <c r="F1497" t="inlineStr">
         <is>
-          <t>Madagascar</t>
+          <t>Gambia</t>
         </is>
       </c>
     </row>
     <row r="1498">
       <c r="A1498" t="inlineStr">
         <is>
-          <t>GMB</t>
+          <t>ETH</t>
         </is>
       </c>
       <c r="B1498" t="n">
@@ -41135,14 +41135,14 @@
       </c>
       <c r="F1498" t="inlineStr">
         <is>
-          <t>Gambia</t>
+          <t>Ethiopia</t>
         </is>
       </c>
     </row>
     <row r="1499">
       <c r="A1499" t="inlineStr">
         <is>
-          <t>ETH</t>
+          <t>ERI</t>
         </is>
       </c>
       <c r="B1499" t="n">
@@ -41161,14 +41161,14 @@
       </c>
       <c r="F1499" t="inlineStr">
         <is>
-          <t>Ethiopia</t>
+          <t>Eritrea</t>
         </is>
       </c>
     </row>
     <row r="1500">
       <c r="A1500" t="inlineStr">
         <is>
-          <t>ERI</t>
+          <t>GNB</t>
         </is>
       </c>
       <c r="B1500" t="n">
@@ -41187,14 +41187,14 @@
       </c>
       <c r="F1500" t="inlineStr">
         <is>
-          <t>Eritrea</t>
+          <t>Guinea-Bissau</t>
         </is>
       </c>
     </row>
     <row r="1501">
       <c r="A1501" t="inlineStr">
         <is>
-          <t>GNB</t>
+          <t>LBR</t>
         </is>
       </c>
       <c r="B1501" t="n">
@@ -41213,14 +41213,14 @@
       </c>
       <c r="F1501" t="inlineStr">
         <is>
-          <t>Guinea-Bissau</t>
+          <t>Liberia</t>
         </is>
       </c>
     </row>
     <row r="1502">
       <c r="A1502" t="inlineStr">
         <is>
-          <t>LBR</t>
+          <t>COD</t>
         </is>
       </c>
       <c r="B1502" t="n">
@@ -41239,14 +41239,14 @@
       </c>
       <c r="F1502" t="inlineStr">
         <is>
-          <t>Liberia</t>
+          <t>DR Congo</t>
         </is>
       </c>
     </row>
     <row r="1503">
       <c r="A1503" t="inlineStr">
         <is>
-          <t>COD</t>
+          <t>AFG</t>
         </is>
       </c>
       <c r="B1503" t="n">
@@ -41265,14 +41265,14 @@
       </c>
       <c r="F1503" t="inlineStr">
         <is>
-          <t>DR Congo</t>
+          <t>Afghanistan</t>
         </is>
       </c>
     </row>
     <row r="1504">
       <c r="A1504" t="inlineStr">
         <is>
-          <t>AFG</t>
+          <t>SLE</t>
         </is>
       </c>
       <c r="B1504" t="n">
@@ -41291,14 +41291,14 @@
       </c>
       <c r="F1504" t="inlineStr">
         <is>
-          <t>Afghanistan</t>
+          <t>Sierra Leone</t>
         </is>
       </c>
     </row>
     <row r="1505">
       <c r="A1505" t="inlineStr">
         <is>
-          <t>SLE</t>
+          <t>GIN</t>
         </is>
       </c>
       <c r="B1505" t="n">
@@ -41317,14 +41317,14 @@
       </c>
       <c r="F1505" t="inlineStr">
         <is>
-          <t>Sierra Leone</t>
+          <t>Guinea</t>
         </is>
       </c>
     </row>
     <row r="1506">
       <c r="A1506" t="inlineStr">
         <is>
-          <t>GIN</t>
+          <t>YEM</t>
         </is>
       </c>
       <c r="B1506" t="n">
@@ -41343,14 +41343,14 @@
       </c>
       <c r="F1506" t="inlineStr">
         <is>
-          <t>Guinea</t>
+          <t>Yemen</t>
         </is>
       </c>
     </row>
     <row r="1507">
       <c r="A1507" t="inlineStr">
         <is>
-          <t>YEM</t>
+          <t>BFA</t>
         </is>
       </c>
       <c r="B1507" t="n">
@@ -41369,14 +41369,14 @@
       </c>
       <c r="F1507" t="inlineStr">
         <is>
-          <t>Yemen</t>
+          <t>Burkina Faso</t>
         </is>
       </c>
     </row>
     <row r="1508">
       <c r="A1508" t="inlineStr">
         <is>
-          <t>BFA</t>
+          <t>MOZ</t>
         </is>
       </c>
       <c r="B1508" t="n">
@@ -41395,14 +41395,14 @@
       </c>
       <c r="F1508" t="inlineStr">
         <is>
-          <t>Burkina Faso</t>
+          <t>Mozambique</t>
         </is>
       </c>
     </row>
     <row r="1509">
       <c r="A1509" t="inlineStr">
         <is>
-          <t>MOZ</t>
+          <t>MLI</t>
         </is>
       </c>
       <c r="B1509" t="n">
@@ -41421,14 +41421,14 @@
       </c>
       <c r="F1509" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Mali</t>
         </is>
       </c>
     </row>
     <row r="1510">
       <c r="A1510" t="inlineStr">
         <is>
-          <t>MLI</t>
+          <t>BDI</t>
         </is>
       </c>
       <c r="B1510" t="n">
@@ -41447,14 +41447,14 @@
       </c>
       <c r="F1510" t="inlineStr">
         <is>
-          <t>Mali</t>
+          <t>Burundi</t>
         </is>
       </c>
     </row>
     <row r="1511">
       <c r="A1511" t="inlineStr">
         <is>
-          <t>BDI</t>
+          <t>CAF</t>
         </is>
       </c>
       <c r="B1511" t="n">
@@ -41473,14 +41473,14 @@
       </c>
       <c r="F1511" t="inlineStr">
         <is>
-          <t>Burundi</t>
+          <t>Central African Republic</t>
         </is>
       </c>
     </row>
     <row r="1512">
       <c r="A1512" t="inlineStr">
         <is>
-          <t>CAF</t>
+          <t>NER</t>
         </is>
       </c>
       <c r="B1512" t="n">
@@ -41499,14 +41499,14 @@
       </c>
       <c r="F1512" t="inlineStr">
         <is>
-          <t>Central African Republic</t>
+          <t>Niger</t>
         </is>
       </c>
     </row>
     <row r="1513">
       <c r="A1513" t="inlineStr">
         <is>
-          <t>NER</t>
+          <t>TCD</t>
         </is>
       </c>
       <c r="B1513" t="n">
@@ -41525,14 +41525,14 @@
       </c>
       <c r="F1513" t="inlineStr">
         <is>
-          <t>Niger</t>
+          <t>Chad</t>
         </is>
       </c>
     </row>
     <row r="1514">
       <c r="A1514" t="inlineStr">
         <is>
-          <t>TCD</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="B1514" t="n">
@@ -41551,14 +41551,14 @@
       </c>
       <c r="F1514" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>South Sudan</t>
         </is>
       </c>
     </row>
     <row r="1515">
       <c r="A1515" t="inlineStr">
         <is>
-          <t>SSD</t>
+          <t>PRK</t>
         </is>
       </c>
       <c r="B1515" t="n">
@@ -41577,14 +41577,14 @@
       </c>
       <c r="F1515" t="inlineStr">
         <is>
-          <t>South Sudan</t>
+          <t>North Korea</t>
         </is>
       </c>
     </row>
     <row r="1516">
       <c r="A1516" t="inlineStr">
         <is>
-          <t>PRK</t>
+          <t>MCO</t>
         </is>
       </c>
       <c r="B1516" t="n">
@@ -41603,14 +41603,14 @@
       </c>
       <c r="F1516" t="inlineStr">
         <is>
-          <t>North Korea</t>
+          <t>Monaco</t>
         </is>
       </c>
     </row>
     <row r="1517">
       <c r="A1517" t="inlineStr">
         <is>
-          <t>MCO</t>
+          <t>NRU</t>
         </is>
       </c>
       <c r="B1517" t="n">
@@ -41629,14 +41629,14 @@
       </c>
       <c r="F1517" t="inlineStr">
         <is>
-          <t>Monaco</t>
+          <t>Nauru</t>
         </is>
       </c>
     </row>
     <row r="1518">
       <c r="A1518" t="inlineStr">
         <is>
-          <t>NRU</t>
+          <t>SOM</t>
         </is>
       </c>
       <c r="B1518" t="n">
@@ -41654,32 +41654,6 @@
         </is>
       </c>
       <c r="F1518" t="inlineStr">
-        <is>
-          <t>Nauru</t>
-        </is>
-      </c>
-    </row>
-    <row r="1519">
-      <c r="A1519" t="inlineStr">
-        <is>
-          <t>SOM</t>
-        </is>
-      </c>
-      <c r="B1519" t="n">
-        <v>2021</v>
-      </c>
-      <c r="C1519" t="inlineStr">
-        <is>
-          <t>Human Development Index</t>
-        </is>
-      </c>
-      <c r="D1519" t="inlineStr"/>
-      <c r="E1519" t="inlineStr">
-        <is>
-          <t>UNDP Human Development Report</t>
-        </is>
-      </c>
-      <c r="F1519" t="inlineStr">
         <is>
           <t>Somalia</t>
         </is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@3c328da46a8469bddec0d02a5fe4345d355411e6 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -25000,7 +25000,7 @@
         </is>
       </c>
       <c r="B878" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C878" t="inlineStr">
         <is>
@@ -25026,7 +25026,7 @@
         </is>
       </c>
       <c r="B879" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C879" t="inlineStr">
         <is>
@@ -25052,7 +25052,7 @@
         </is>
       </c>
       <c r="B880" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C880" t="inlineStr">
         <is>
@@ -25078,7 +25078,7 @@
         </is>
       </c>
       <c r="B881" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C881" t="inlineStr">
         <is>
@@ -25104,7 +25104,7 @@
         </is>
       </c>
       <c r="B882" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C882" t="inlineStr">
         <is>
@@ -25130,7 +25130,7 @@
         </is>
       </c>
       <c r="B883" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C883" t="inlineStr">
         <is>
@@ -25156,7 +25156,7 @@
         </is>
       </c>
       <c r="B884" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C884" t="inlineStr">
         <is>
@@ -25182,7 +25182,7 @@
         </is>
       </c>
       <c r="B885" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C885" t="inlineStr">
         <is>
@@ -25208,7 +25208,7 @@
         </is>
       </c>
       <c r="B886" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C886" t="inlineStr">
         <is>
@@ -25234,7 +25234,7 @@
         </is>
       </c>
       <c r="B887" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C887" t="inlineStr">
         <is>
@@ -25260,7 +25260,7 @@
         </is>
       </c>
       <c r="B888" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C888" t="inlineStr">
         <is>
@@ -25286,7 +25286,7 @@
         </is>
       </c>
       <c r="B889" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C889" t="inlineStr">
         <is>
@@ -25312,7 +25312,7 @@
         </is>
       </c>
       <c r="B890" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C890" t="inlineStr">
         <is>
@@ -25338,7 +25338,7 @@
         </is>
       </c>
       <c r="B891" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C891" t="inlineStr">
         <is>
@@ -25364,7 +25364,7 @@
         </is>
       </c>
       <c r="B892" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C892" t="inlineStr">
         <is>
@@ -25390,7 +25390,7 @@
         </is>
       </c>
       <c r="B893" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C893" t="inlineStr">
         <is>
@@ -25416,7 +25416,7 @@
         </is>
       </c>
       <c r="B894" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C894" t="inlineStr">
         <is>
@@ -25442,7 +25442,7 @@
         </is>
       </c>
       <c r="B895" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C895" t="inlineStr">
         <is>
@@ -25468,7 +25468,7 @@
         </is>
       </c>
       <c r="B896" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C896" t="inlineStr">
         <is>
@@ -25494,7 +25494,7 @@
         </is>
       </c>
       <c r="B897" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C897" t="inlineStr">
         <is>
@@ -25520,7 +25520,7 @@
         </is>
       </c>
       <c r="B898" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C898" t="inlineStr">
         <is>
@@ -25546,7 +25546,7 @@
         </is>
       </c>
       <c r="B899" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C899" t="inlineStr">
         <is>
@@ -25572,7 +25572,7 @@
         </is>
       </c>
       <c r="B900" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C900" t="inlineStr">
         <is>
@@ -25598,7 +25598,7 @@
         </is>
       </c>
       <c r="B901" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C901" t="inlineStr">
         <is>
@@ -25624,7 +25624,7 @@
         </is>
       </c>
       <c r="B902" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C902" t="inlineStr">
         <is>
@@ -25650,7 +25650,7 @@
         </is>
       </c>
       <c r="B903" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C903" t="inlineStr">
         <is>
@@ -25676,7 +25676,7 @@
         </is>
       </c>
       <c r="B904" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C904" t="inlineStr">
         <is>
@@ -25702,7 +25702,7 @@
         </is>
       </c>
       <c r="B905" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C905" t="inlineStr">
         <is>
@@ -25728,7 +25728,7 @@
         </is>
       </c>
       <c r="B906" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C906" t="inlineStr">
         <is>
@@ -25754,7 +25754,7 @@
         </is>
       </c>
       <c r="B907" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C907" t="inlineStr">
         <is>
@@ -25780,7 +25780,7 @@
         </is>
       </c>
       <c r="B908" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C908" t="inlineStr">
         <is>
@@ -25806,7 +25806,7 @@
         </is>
       </c>
       <c r="B909" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C909" t="inlineStr">
         <is>
@@ -25832,7 +25832,7 @@
         </is>
       </c>
       <c r="B910" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C910" t="inlineStr">
         <is>
@@ -25858,7 +25858,7 @@
         </is>
       </c>
       <c r="B911" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C911" t="inlineStr">
         <is>
@@ -25884,7 +25884,7 @@
         </is>
       </c>
       <c r="B912" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C912" t="inlineStr">
         <is>
@@ -25910,7 +25910,7 @@
         </is>
       </c>
       <c r="B913" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C913" t="inlineStr">
         <is>
@@ -25936,7 +25936,7 @@
         </is>
       </c>
       <c r="B914" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C914" t="inlineStr">
         <is>
@@ -25962,7 +25962,7 @@
         </is>
       </c>
       <c r="B915" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C915" t="inlineStr">
         <is>
@@ -25988,7 +25988,7 @@
         </is>
       </c>
       <c r="B916" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C916" t="inlineStr">
         <is>
@@ -26014,7 +26014,7 @@
         </is>
       </c>
       <c r="B917" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C917" t="inlineStr">
         <is>
@@ -26040,7 +26040,7 @@
         </is>
       </c>
       <c r="B918" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C918" t="inlineStr">
         <is>
@@ -26066,7 +26066,7 @@
         </is>
       </c>
       <c r="B919" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C919" t="inlineStr">
         <is>
@@ -26092,7 +26092,7 @@
         </is>
       </c>
       <c r="B920" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C920" t="inlineStr">
         <is>
@@ -26118,7 +26118,7 @@
         </is>
       </c>
       <c r="B921" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C921" t="inlineStr">
         <is>
@@ -26144,7 +26144,7 @@
         </is>
       </c>
       <c r="B922" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C922" t="inlineStr">
         <is>
@@ -26170,7 +26170,7 @@
         </is>
       </c>
       <c r="B923" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C923" t="inlineStr">
         <is>
@@ -26196,7 +26196,7 @@
         </is>
       </c>
       <c r="B924" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C924" t="inlineStr">
         <is>
@@ -26222,7 +26222,7 @@
         </is>
       </c>
       <c r="B925" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C925" t="inlineStr">
         <is>
@@ -26248,7 +26248,7 @@
         </is>
       </c>
       <c r="B926" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C926" t="inlineStr">
         <is>
@@ -26274,7 +26274,7 @@
         </is>
       </c>
       <c r="B927" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C927" t="inlineStr">
         <is>
@@ -26300,7 +26300,7 @@
         </is>
       </c>
       <c r="B928" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C928" t="inlineStr">
         <is>
@@ -26326,7 +26326,7 @@
         </is>
       </c>
       <c r="B929" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C929" t="inlineStr">
         <is>
@@ -26352,7 +26352,7 @@
         </is>
       </c>
       <c r="B930" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C930" t="inlineStr">
         <is>
@@ -26378,7 +26378,7 @@
         </is>
       </c>
       <c r="B931" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C931" t="inlineStr">
         <is>
@@ -26404,7 +26404,7 @@
         </is>
       </c>
       <c r="B932" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C932" t="inlineStr">
         <is>
@@ -26430,7 +26430,7 @@
         </is>
       </c>
       <c r="B933" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C933" t="inlineStr">
         <is>
@@ -26456,7 +26456,7 @@
         </is>
       </c>
       <c r="B934" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C934" t="inlineStr">
         <is>
@@ -26482,7 +26482,7 @@
         </is>
       </c>
       <c r="B935" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C935" t="inlineStr">
         <is>
@@ -26508,7 +26508,7 @@
         </is>
       </c>
       <c r="B936" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C936" t="inlineStr">
         <is>
@@ -26534,7 +26534,7 @@
         </is>
       </c>
       <c r="B937" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C937" t="inlineStr">
         <is>
@@ -26560,7 +26560,7 @@
         </is>
       </c>
       <c r="B938" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C938" t="inlineStr">
         <is>
@@ -26586,7 +26586,7 @@
         </is>
       </c>
       <c r="B939" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C939" t="inlineStr">
         <is>
@@ -26612,7 +26612,7 @@
         </is>
       </c>
       <c r="B940" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C940" t="inlineStr">
         <is>
@@ -26638,7 +26638,7 @@
         </is>
       </c>
       <c r="B941" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C941" t="inlineStr">
         <is>
@@ -26664,7 +26664,7 @@
         </is>
       </c>
       <c r="B942" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C942" t="inlineStr">
         <is>
@@ -26690,7 +26690,7 @@
         </is>
       </c>
       <c r="B943" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C943" t="inlineStr">
         <is>
@@ -26716,7 +26716,7 @@
         </is>
       </c>
       <c r="B944" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C944" t="inlineStr">
         <is>
@@ -26742,7 +26742,7 @@
         </is>
       </c>
       <c r="B945" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C945" t="inlineStr">
         <is>
@@ -26768,7 +26768,7 @@
         </is>
       </c>
       <c r="B946" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C946" t="inlineStr">
         <is>
@@ -26794,7 +26794,7 @@
         </is>
       </c>
       <c r="B947" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C947" t="inlineStr">
         <is>
@@ -26820,7 +26820,7 @@
         </is>
       </c>
       <c r="B948" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C948" t="inlineStr">
         <is>
@@ -26846,7 +26846,7 @@
         </is>
       </c>
       <c r="B949" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C949" t="inlineStr">
         <is>
@@ -26872,7 +26872,7 @@
         </is>
       </c>
       <c r="B950" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C950" t="inlineStr">
         <is>
@@ -26898,7 +26898,7 @@
         </is>
       </c>
       <c r="B951" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C951" t="inlineStr">
         <is>
@@ -26924,7 +26924,7 @@
         </is>
       </c>
       <c r="B952" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C952" t="inlineStr">
         <is>
@@ -26950,7 +26950,7 @@
         </is>
       </c>
       <c r="B953" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C953" t="inlineStr">
         <is>
@@ -26976,7 +26976,7 @@
         </is>
       </c>
       <c r="B954" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C954" t="inlineStr">
         <is>
@@ -27002,7 +27002,7 @@
         </is>
       </c>
       <c r="B955" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C955" t="inlineStr">
         <is>
@@ -27028,7 +27028,7 @@
         </is>
       </c>
       <c r="B956" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C956" t="inlineStr">
         <is>
@@ -27054,7 +27054,7 @@
         </is>
       </c>
       <c r="B957" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C957" t="inlineStr">
         <is>
@@ -27080,7 +27080,7 @@
         </is>
       </c>
       <c r="B958" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C958" t="inlineStr">
         <is>
@@ -27106,7 +27106,7 @@
         </is>
       </c>
       <c r="B959" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C959" t="inlineStr">
         <is>
@@ -27132,7 +27132,7 @@
         </is>
       </c>
       <c r="B960" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C960" t="inlineStr">
         <is>
@@ -27158,7 +27158,7 @@
         </is>
       </c>
       <c r="B961" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C961" t="inlineStr">
         <is>
@@ -27184,7 +27184,7 @@
         </is>
       </c>
       <c r="B962" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C962" t="inlineStr">
         <is>
@@ -27210,7 +27210,7 @@
         </is>
       </c>
       <c r="B963" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C963" t="inlineStr">
         <is>
@@ -27236,7 +27236,7 @@
         </is>
       </c>
       <c r="B964" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C964" t="inlineStr">
         <is>
@@ -27262,7 +27262,7 @@
         </is>
       </c>
       <c r="B965" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C965" t="inlineStr">
         <is>
@@ -27288,7 +27288,7 @@
         </is>
       </c>
       <c r="B966" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C966" t="inlineStr">
         <is>
@@ -27314,7 +27314,7 @@
         </is>
       </c>
       <c r="B967" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C967" t="inlineStr">
         <is>
@@ -27340,7 +27340,7 @@
         </is>
       </c>
       <c r="B968" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C968" t="inlineStr">
         <is>
@@ -27366,7 +27366,7 @@
         </is>
       </c>
       <c r="B969" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C969" t="inlineStr">
         <is>
@@ -27392,7 +27392,7 @@
         </is>
       </c>
       <c r="B970" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C970" t="inlineStr">
         <is>
@@ -27418,7 +27418,7 @@
         </is>
       </c>
       <c r="B971" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C971" t="inlineStr">
         <is>
@@ -27444,7 +27444,7 @@
         </is>
       </c>
       <c r="B972" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C972" t="inlineStr">
         <is>
@@ -27470,7 +27470,7 @@
         </is>
       </c>
       <c r="B973" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C973" t="inlineStr">
         <is>
@@ -27496,7 +27496,7 @@
         </is>
       </c>
       <c r="B974" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C974" t="inlineStr">
         <is>
@@ -27522,7 +27522,7 @@
         </is>
       </c>
       <c r="B975" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C975" t="inlineStr">
         <is>
@@ -27548,7 +27548,7 @@
         </is>
       </c>
       <c r="B976" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C976" t="inlineStr">
         <is>
@@ -27574,7 +27574,7 @@
         </is>
       </c>
       <c r="B977" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C977" t="inlineStr">
         <is>
@@ -27600,7 +27600,7 @@
         </is>
       </c>
       <c r="B978" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C978" t="inlineStr">
         <is>
@@ -27626,7 +27626,7 @@
         </is>
       </c>
       <c r="B979" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C979" t="inlineStr">
         <is>
@@ -27652,7 +27652,7 @@
         </is>
       </c>
       <c r="B980" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C980" t="inlineStr">
         <is>
@@ -27678,7 +27678,7 @@
         </is>
       </c>
       <c r="B981" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C981" t="inlineStr">
         <is>
@@ -27704,7 +27704,7 @@
         </is>
       </c>
       <c r="B982" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C982" t="inlineStr">
         <is>
@@ -27730,7 +27730,7 @@
         </is>
       </c>
       <c r="B983" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C983" t="inlineStr">
         <is>
@@ -27756,7 +27756,7 @@
         </is>
       </c>
       <c r="B984" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C984" t="inlineStr">
         <is>
@@ -27782,7 +27782,7 @@
         </is>
       </c>
       <c r="B985" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C985" t="inlineStr">
         <is>
@@ -27808,7 +27808,7 @@
         </is>
       </c>
       <c r="B986" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C986" t="inlineStr">
         <is>
@@ -27834,7 +27834,7 @@
         </is>
       </c>
       <c r="B987" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C987" t="inlineStr">
         <is>
@@ -27860,7 +27860,7 @@
         </is>
       </c>
       <c r="B988" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C988" t="inlineStr">
         <is>
@@ -27886,7 +27886,7 @@
         </is>
       </c>
       <c r="B989" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C989" t="inlineStr">
         <is>
@@ -27912,7 +27912,7 @@
         </is>
       </c>
       <c r="B990" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C990" t="inlineStr">
         <is>
@@ -27938,7 +27938,7 @@
         </is>
       </c>
       <c r="B991" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C991" t="inlineStr">
         <is>
@@ -27964,7 +27964,7 @@
         </is>
       </c>
       <c r="B992" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C992" t="inlineStr">
         <is>
@@ -27990,7 +27990,7 @@
         </is>
       </c>
       <c r="B993" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C993" t="inlineStr">
         <is>
@@ -28016,7 +28016,7 @@
         </is>
       </c>
       <c r="B994" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C994" t="inlineStr">
         <is>
@@ -28042,7 +28042,7 @@
         </is>
       </c>
       <c r="B995" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C995" t="inlineStr">
         <is>
@@ -28068,7 +28068,7 @@
         </is>
       </c>
       <c r="B996" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C996" t="inlineStr">
         <is>
@@ -28094,7 +28094,7 @@
         </is>
       </c>
       <c r="B997" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C997" t="inlineStr">
         <is>
@@ -28120,7 +28120,7 @@
         </is>
       </c>
       <c r="B998" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C998" t="inlineStr">
         <is>
@@ -28146,7 +28146,7 @@
         </is>
       </c>
       <c r="B999" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C999" t="inlineStr">
         <is>
@@ -28172,7 +28172,7 @@
         </is>
       </c>
       <c r="B1000" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1000" t="inlineStr">
         <is>
@@ -28198,7 +28198,7 @@
         </is>
       </c>
       <c r="B1001" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1001" t="inlineStr">
         <is>
@@ -28224,7 +28224,7 @@
         </is>
       </c>
       <c r="B1002" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1002" t="inlineStr">
         <is>
@@ -28250,7 +28250,7 @@
         </is>
       </c>
       <c r="B1003" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1003" t="inlineStr">
         <is>
@@ -28276,7 +28276,7 @@
         </is>
       </c>
       <c r="B1004" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1004" t="inlineStr">
         <is>
@@ -28302,7 +28302,7 @@
         </is>
       </c>
       <c r="B1005" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1005" t="inlineStr">
         <is>
@@ -28328,7 +28328,7 @@
         </is>
       </c>
       <c r="B1006" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1006" t="inlineStr">
         <is>
@@ -28354,7 +28354,7 @@
         </is>
       </c>
       <c r="B1007" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1007" t="inlineStr">
         <is>
@@ -28380,7 +28380,7 @@
         </is>
       </c>
       <c r="B1008" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1008" t="inlineStr">
         <is>
@@ -28406,7 +28406,7 @@
         </is>
       </c>
       <c r="B1009" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1009" t="inlineStr">
         <is>
@@ -28432,7 +28432,7 @@
         </is>
       </c>
       <c r="B1010" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1010" t="inlineStr">
         <is>
@@ -28458,7 +28458,7 @@
         </is>
       </c>
       <c r="B1011" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1011" t="inlineStr">
         <is>
@@ -28484,7 +28484,7 @@
         </is>
       </c>
       <c r="B1012" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1012" t="inlineStr">
         <is>
@@ -28510,7 +28510,7 @@
         </is>
       </c>
       <c r="B1013" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1013" t="inlineStr">
         <is>
@@ -28536,7 +28536,7 @@
         </is>
       </c>
       <c r="B1014" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1014" t="inlineStr">
         <is>
@@ -28562,7 +28562,7 @@
         </is>
       </c>
       <c r="B1015" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1015" t="inlineStr">
         <is>
@@ -28588,7 +28588,7 @@
         </is>
       </c>
       <c r="B1016" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1016" t="inlineStr">
         <is>
@@ -28614,7 +28614,7 @@
         </is>
       </c>
       <c r="B1017" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1017" t="inlineStr">
         <is>
@@ -28640,7 +28640,7 @@
         </is>
       </c>
       <c r="B1018" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1018" t="inlineStr">
         <is>
@@ -28666,7 +28666,7 @@
         </is>
       </c>
       <c r="B1019" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1019" t="inlineStr">
         <is>
@@ -28692,7 +28692,7 @@
         </is>
       </c>
       <c r="B1020" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1020" t="inlineStr">
         <is>
@@ -28718,7 +28718,7 @@
         </is>
       </c>
       <c r="B1021" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1021" t="inlineStr">
         <is>
@@ -28744,7 +28744,7 @@
         </is>
       </c>
       <c r="B1022" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1022" t="inlineStr">
         <is>
@@ -28770,7 +28770,7 @@
         </is>
       </c>
       <c r="B1023" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1023" t="inlineStr">
         <is>
@@ -28796,7 +28796,7 @@
         </is>
       </c>
       <c r="B1024" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1024" t="inlineStr">
         <is>
@@ -28822,7 +28822,7 @@
         </is>
       </c>
       <c r="B1025" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1025" t="inlineStr">
         <is>
@@ -28848,7 +28848,7 @@
         </is>
       </c>
       <c r="B1026" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1026" t="inlineStr">
         <is>
@@ -28874,7 +28874,7 @@
         </is>
       </c>
       <c r="B1027" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1027" t="inlineStr">
         <is>
@@ -28900,7 +28900,7 @@
         </is>
       </c>
       <c r="B1028" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1028" t="inlineStr">
         <is>
@@ -28926,7 +28926,7 @@
         </is>
       </c>
       <c r="B1029" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1029" t="inlineStr">
         <is>
@@ -28952,7 +28952,7 @@
         </is>
       </c>
       <c r="B1030" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1030" t="inlineStr">
         <is>
@@ -28978,7 +28978,7 @@
         </is>
       </c>
       <c r="B1031" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1031" t="inlineStr">
         <is>
@@ -29004,7 +29004,7 @@
         </is>
       </c>
       <c r="B1032" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1032" t="inlineStr">
         <is>
@@ -29030,7 +29030,7 @@
         </is>
       </c>
       <c r="B1033" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1033" t="inlineStr">
         <is>
@@ -29056,7 +29056,7 @@
         </is>
       </c>
       <c r="B1034" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1034" t="inlineStr">
         <is>
@@ -29082,7 +29082,7 @@
         </is>
       </c>
       <c r="B1035" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1035" t="inlineStr">
         <is>
@@ -29108,7 +29108,7 @@
         </is>
       </c>
       <c r="B1036" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1036" t="inlineStr">
         <is>
@@ -29134,7 +29134,7 @@
         </is>
       </c>
       <c r="B1037" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1037" t="inlineStr">
         <is>
@@ -29160,7 +29160,7 @@
         </is>
       </c>
       <c r="B1038" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1038" t="inlineStr">
         <is>
@@ -29186,7 +29186,7 @@
         </is>
       </c>
       <c r="B1039" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1039" t="inlineStr">
         <is>
@@ -29212,7 +29212,7 @@
         </is>
       </c>
       <c r="B1040" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1040" t="inlineStr">
         <is>
@@ -29238,7 +29238,7 @@
         </is>
       </c>
       <c r="B1041" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1041" t="inlineStr">
         <is>
@@ -29264,7 +29264,7 @@
         </is>
       </c>
       <c r="B1042" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1042" t="inlineStr">
         <is>
@@ -29290,7 +29290,7 @@
         </is>
       </c>
       <c r="B1043" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1043" t="inlineStr">
         <is>
@@ -29316,7 +29316,7 @@
         </is>
       </c>
       <c r="B1044" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1044" t="inlineStr">
         <is>
@@ -29342,7 +29342,7 @@
         </is>
       </c>
       <c r="B1045" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1045" t="inlineStr">
         <is>
@@ -29368,7 +29368,7 @@
         </is>
       </c>
       <c r="B1046" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1046" t="inlineStr">
         <is>
@@ -29394,7 +29394,7 @@
         </is>
       </c>
       <c r="B1047" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1047" t="inlineStr">
         <is>
@@ -29420,7 +29420,7 @@
         </is>
       </c>
       <c r="B1048" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1048" t="inlineStr">
         <is>
@@ -29446,7 +29446,7 @@
         </is>
       </c>
       <c r="B1049" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1049" t="inlineStr">
         <is>
@@ -29472,7 +29472,7 @@
         </is>
       </c>
       <c r="B1050" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1050" t="inlineStr">
         <is>
@@ -29498,7 +29498,7 @@
         </is>
       </c>
       <c r="B1051" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1051" t="inlineStr">
         <is>
@@ -29524,7 +29524,7 @@
         </is>
       </c>
       <c r="B1052" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1052" t="inlineStr">
         <is>
@@ -29550,7 +29550,7 @@
         </is>
       </c>
       <c r="B1053" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1053" t="inlineStr">
         <is>
@@ -29576,7 +29576,7 @@
         </is>
       </c>
       <c r="B1054" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1054" t="inlineStr">
         <is>
@@ -29602,7 +29602,7 @@
         </is>
       </c>
       <c r="B1055" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1055" t="inlineStr">
         <is>
@@ -29628,7 +29628,7 @@
         </is>
       </c>
       <c r="B1056" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1056" t="inlineStr">
         <is>
@@ -29654,7 +29654,7 @@
         </is>
       </c>
       <c r="B1057" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1057" t="inlineStr">
         <is>
@@ -29680,7 +29680,7 @@
         </is>
       </c>
       <c r="B1058" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1058" t="inlineStr">
         <is>
@@ -29706,7 +29706,7 @@
         </is>
       </c>
       <c r="B1059" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1059" t="inlineStr">
         <is>
@@ -29732,7 +29732,7 @@
         </is>
       </c>
       <c r="B1060" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1060" t="inlineStr">
         <is>
@@ -29758,7 +29758,7 @@
         </is>
       </c>
       <c r="B1061" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1061" t="inlineStr">
         <is>
@@ -29784,7 +29784,7 @@
         </is>
       </c>
       <c r="B1062" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1062" t="inlineStr">
         <is>
@@ -29810,7 +29810,7 @@
         </is>
       </c>
       <c r="B1063" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1063" t="inlineStr">
         <is>
@@ -29836,7 +29836,7 @@
         </is>
       </c>
       <c r="B1064" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1064" t="inlineStr">
         <is>
@@ -29862,7 +29862,7 @@
         </is>
       </c>
       <c r="B1065" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1065" t="inlineStr">
         <is>
@@ -29888,7 +29888,7 @@
         </is>
       </c>
       <c r="B1066" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1066" t="inlineStr">
         <is>
@@ -29914,7 +29914,7 @@
         </is>
       </c>
       <c r="B1067" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1067" t="inlineStr">
         <is>
@@ -29940,7 +29940,7 @@
         </is>
       </c>
       <c r="B1068" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1068" t="inlineStr">
         <is>
@@ -29966,7 +29966,7 @@
         </is>
       </c>
       <c r="B1069" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1069" t="inlineStr">
         <is>
@@ -29992,7 +29992,7 @@
         </is>
       </c>
       <c r="B1070" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1070" t="inlineStr">
         <is>
@@ -30018,7 +30018,7 @@
         </is>
       </c>
       <c r="B1071" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1071" t="inlineStr">
         <is>
@@ -30044,7 +30044,7 @@
         </is>
       </c>
       <c r="B1072" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1072" t="inlineStr">
         <is>
@@ -30070,7 +30070,7 @@
         </is>
       </c>
       <c r="B1073" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1073" t="inlineStr">
         <is>
@@ -30096,7 +30096,7 @@
         </is>
       </c>
       <c r="B1074" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1074" t="inlineStr">
         <is>
@@ -30122,7 +30122,7 @@
         </is>
       </c>
       <c r="B1075" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1075" t="inlineStr">
         <is>
@@ -30148,7 +30148,7 @@
         </is>
       </c>
       <c r="B1076" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1076" t="inlineStr">
         <is>
@@ -30174,7 +30174,7 @@
         </is>
       </c>
       <c r="B1077" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1077" t="inlineStr">
         <is>
@@ -30200,7 +30200,7 @@
         </is>
       </c>
       <c r="B1078" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1078" t="inlineStr">
         <is>
@@ -30226,7 +30226,7 @@
         </is>
       </c>
       <c r="B1079" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1079" t="inlineStr">
         <is>
@@ -30252,7 +30252,7 @@
         </is>
       </c>
       <c r="B1080" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1080" t="inlineStr">
         <is>
@@ -30278,7 +30278,7 @@
         </is>
       </c>
       <c r="B1081" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1081" t="inlineStr">
         <is>
@@ -30304,7 +30304,7 @@
         </is>
       </c>
       <c r="B1082" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1082" t="inlineStr">
         <is>
@@ -30330,7 +30330,7 @@
         </is>
       </c>
       <c r="B1083" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1083" t="inlineStr">
         <is>
@@ -30356,7 +30356,7 @@
         </is>
       </c>
       <c r="B1084" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1084" t="inlineStr">
         <is>
@@ -30382,7 +30382,7 @@
         </is>
       </c>
       <c r="B1085" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1085" t="inlineStr">
         <is>
@@ -30408,7 +30408,7 @@
         </is>
       </c>
       <c r="B1086" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1086" t="inlineStr">
         <is>
@@ -30434,7 +30434,7 @@
         </is>
       </c>
       <c r="B1087" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1087" t="inlineStr">
         <is>
@@ -30460,7 +30460,7 @@
         </is>
       </c>
       <c r="B1088" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1088" t="inlineStr">
         <is>
@@ -30486,7 +30486,7 @@
         </is>
       </c>
       <c r="B1089" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1089" t="inlineStr">
         <is>
@@ -30512,7 +30512,7 @@
         </is>
       </c>
       <c r="B1090" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1090" t="inlineStr">
         <is>
@@ -30538,7 +30538,7 @@
         </is>
       </c>
       <c r="B1091" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1091" t="inlineStr">
         <is>
@@ -30564,7 +30564,7 @@
         </is>
       </c>
       <c r="B1092" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1092" t="inlineStr">
         <is>
@@ -30590,7 +30590,7 @@
         </is>
       </c>
       <c r="B1093" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1093" t="inlineStr">
         <is>
@@ -30616,7 +30616,7 @@
         </is>
       </c>
       <c r="B1094" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1094" t="inlineStr">
         <is>
@@ -30642,7 +30642,7 @@
         </is>
       </c>
       <c r="B1095" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1095" t="inlineStr">
         <is>
@@ -30668,7 +30668,7 @@
         </is>
       </c>
       <c r="B1096" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1096" t="inlineStr">
         <is>
@@ -30694,7 +30694,7 @@
         </is>
       </c>
       <c r="B1097" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1097" t="inlineStr">
         <is>
@@ -30720,7 +30720,7 @@
         </is>
       </c>
       <c r="B1098" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1098" t="inlineStr">
         <is>
@@ -30746,7 +30746,7 @@
         </is>
       </c>
       <c r="B1099" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1099" t="inlineStr">
         <is>
@@ -30772,7 +30772,7 @@
         </is>
       </c>
       <c r="B1100" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1100" t="inlineStr">
         <is>
@@ -30798,7 +30798,7 @@
         </is>
       </c>
       <c r="B1101" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1101" t="inlineStr">
         <is>
@@ -30824,7 +30824,7 @@
         </is>
       </c>
       <c r="B1102" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1102" t="inlineStr">
         <is>
@@ -30850,7 +30850,7 @@
         </is>
       </c>
       <c r="B1103" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1103" t="inlineStr">
         <is>
@@ -30876,7 +30876,7 @@
         </is>
       </c>
       <c r="B1104" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1104" t="inlineStr">
         <is>
@@ -30902,7 +30902,7 @@
         </is>
       </c>
       <c r="B1105" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1105" t="inlineStr">
         <is>
@@ -30928,7 +30928,7 @@
         </is>
       </c>
       <c r="B1106" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1106" t="inlineStr">
         <is>
@@ -30954,7 +30954,7 @@
         </is>
       </c>
       <c r="B1107" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1107" t="inlineStr">
         <is>
@@ -30980,7 +30980,7 @@
         </is>
       </c>
       <c r="B1108" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1108" t="inlineStr">
         <is>
@@ -31006,7 +31006,7 @@
         </is>
       </c>
       <c r="B1109" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1109" t="inlineStr">
         <is>
@@ -31032,7 +31032,7 @@
         </is>
       </c>
       <c r="B1110" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1110" t="inlineStr">
         <is>
@@ -31058,7 +31058,7 @@
         </is>
       </c>
       <c r="B1111" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1111" t="inlineStr">
         <is>
@@ -31084,7 +31084,7 @@
         </is>
       </c>
       <c r="B1112" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1112" t="inlineStr">
         <is>
@@ -31110,7 +31110,7 @@
         </is>
       </c>
       <c r="B1113" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1113" t="inlineStr">
         <is>
@@ -31136,7 +31136,7 @@
         </is>
       </c>
       <c r="B1114" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1114" t="inlineStr">
         <is>
@@ -31162,7 +31162,7 @@
         </is>
       </c>
       <c r="B1115" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1115" t="inlineStr">
         <is>
@@ -31188,7 +31188,7 @@
         </is>
       </c>
       <c r="B1116" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1116" t="inlineStr">
         <is>
@@ -31214,7 +31214,7 @@
         </is>
       </c>
       <c r="B1117" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1117" t="inlineStr">
         <is>
@@ -31240,7 +31240,7 @@
         </is>
       </c>
       <c r="B1118" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1118" t="inlineStr">
         <is>
@@ -31266,7 +31266,7 @@
         </is>
       </c>
       <c r="B1119" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1119" t="inlineStr">
         <is>
@@ -31292,7 +31292,7 @@
         </is>
       </c>
       <c r="B1120" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1120" t="inlineStr">
         <is>
@@ -31318,7 +31318,7 @@
         </is>
       </c>
       <c r="B1121" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1121" t="inlineStr">
         <is>
@@ -31344,7 +31344,7 @@
         </is>
       </c>
       <c r="B1122" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1122" t="inlineStr">
         <is>
@@ -31370,7 +31370,7 @@
         </is>
       </c>
       <c r="B1123" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1123" t="inlineStr">
         <is>
@@ -31396,7 +31396,7 @@
         </is>
       </c>
       <c r="B1124" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1124" t="inlineStr">
         <is>
@@ -31422,7 +31422,7 @@
         </is>
       </c>
       <c r="B1125" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1125" t="inlineStr">
         <is>
@@ -31448,7 +31448,7 @@
         </is>
       </c>
       <c r="B1126" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1126" t="inlineStr">
         <is>
@@ -31474,7 +31474,7 @@
         </is>
       </c>
       <c r="B1127" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1127" t="inlineStr">
         <is>
@@ -31500,7 +31500,7 @@
         </is>
       </c>
       <c r="B1128" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1128" t="inlineStr">
         <is>
@@ -31526,7 +31526,7 @@
         </is>
       </c>
       <c r="B1129" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1129" t="inlineStr">
         <is>
@@ -31552,7 +31552,7 @@
         </is>
       </c>
       <c r="B1130" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1130" t="inlineStr">
         <is>
@@ -31578,7 +31578,7 @@
         </is>
       </c>
       <c r="B1131" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1131" t="inlineStr">
         <is>
@@ -31604,7 +31604,7 @@
         </is>
       </c>
       <c r="B1132" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1132" t="inlineStr">
         <is>
@@ -31630,7 +31630,7 @@
         </is>
       </c>
       <c r="B1133" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1133" t="inlineStr">
         <is>
@@ -31656,7 +31656,7 @@
         </is>
       </c>
       <c r="B1134" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1134" t="inlineStr">
         <is>
@@ -31682,7 +31682,7 @@
         </is>
       </c>
       <c r="B1135" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1135" t="inlineStr">
         <is>
@@ -31708,7 +31708,7 @@
         </is>
       </c>
       <c r="B1136" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1136" t="inlineStr">
         <is>
@@ -31734,7 +31734,7 @@
         </is>
       </c>
       <c r="B1137" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1137" t="inlineStr">
         <is>
@@ -31760,7 +31760,7 @@
         </is>
       </c>
       <c r="B1138" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1138" t="inlineStr">
         <is>
@@ -31786,7 +31786,7 @@
         </is>
       </c>
       <c r="B1139" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1139" t="inlineStr">
         <is>
@@ -31812,7 +31812,7 @@
         </is>
       </c>
       <c r="B1140" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1140" t="inlineStr">
         <is>
@@ -31838,7 +31838,7 @@
         </is>
       </c>
       <c r="B1141" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1141" t="inlineStr">
         <is>
@@ -31864,7 +31864,7 @@
         </is>
       </c>
       <c r="B1142" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1142" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@3bd4c66620e75c632e2a2365b88f559711fd4ab0 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -32202,7 +32202,7 @@
         </is>
       </c>
       <c r="B1155" t="n">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="C1155" t="inlineStr">
         <is>
@@ -32384,7 +32384,7 @@
         </is>
       </c>
       <c r="B1162" t="n">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="C1162" t="inlineStr">
         <is>
@@ -32436,7 +32436,7 @@
         </is>
       </c>
       <c r="B1164" t="n">
-        <v>2008</v>
+        <v>2021</v>
       </c>
       <c r="C1164" t="inlineStr">
         <is>
@@ -32462,7 +32462,7 @@
         </is>
       </c>
       <c r="B1165" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C1165" t="inlineStr">
         <is>
@@ -32540,7 +32540,7 @@
         </is>
       </c>
       <c r="B1168" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1168" t="inlineStr">
         <is>
@@ -32748,7 +32748,7 @@
         </is>
       </c>
       <c r="B1176" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1176" t="inlineStr">
         <is>
@@ -32956,7 +32956,7 @@
         </is>
       </c>
       <c r="B1184" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1184" t="inlineStr">
         <is>
@@ -33008,7 +33008,7 @@
         </is>
       </c>
       <c r="B1186" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1186" t="inlineStr">
         <is>
@@ -33528,7 +33528,7 @@
         </is>
       </c>
       <c r="B1206" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C1206" t="inlineStr">
         <is>
@@ -33710,7 +33710,7 @@
         </is>
       </c>
       <c r="B1213" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1213" t="inlineStr">
         <is>
@@ -33996,7 +33996,7 @@
         </is>
       </c>
       <c r="B1224" t="n">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="C1224" t="inlineStr">
         <is>
@@ -34230,7 +34230,7 @@
         </is>
       </c>
       <c r="B1233" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C1233" t="inlineStr">
         <is>
@@ -34282,7 +34282,7 @@
         </is>
       </c>
       <c r="B1235" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1235" t="inlineStr">
         <is>
@@ -34308,7 +34308,7 @@
         </is>
       </c>
       <c r="B1236" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1236" t="inlineStr">
         <is>
@@ -34776,7 +34776,7 @@
         </is>
       </c>
       <c r="B1254" t="n">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="C1254" t="inlineStr">
         <is>
@@ -35296,7 +35296,7 @@
         </is>
       </c>
       <c r="B1274" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1274" t="inlineStr">
         <is>
@@ -35426,7 +35426,7 @@
         </is>
       </c>
       <c r="B1279" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C1279" t="inlineStr">
         <is>
@@ -35556,7 +35556,7 @@
         </is>
       </c>
       <c r="B1284" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1284" t="inlineStr">
         <is>
@@ -36232,7 +36232,7 @@
         </is>
       </c>
       <c r="B1310" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1310" t="inlineStr">
         <is>
@@ -36284,7 +36284,7 @@
         </is>
       </c>
       <c r="B1312" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C1312" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@780b23ea3079b4ae7577b4cdbec11c47b52ebb9a 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -1665,7 +1665,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -7041,7 +7041,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -12025,7 +12025,7 @@
       </c>
       <c r="F414" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -15413,7 +15413,7 @@
       </c>
       <c r="F535" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -20817,7 +20817,7 @@
       </c>
       <c r="F728" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -26447,7 +26447,7 @@
       </c>
       <c r="F933" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -27071,7 +27071,7 @@
       </c>
       <c r="F957" t="inlineStr">
         <is>
-          <t>Faeroe Islands</t>
+          <t>Faroe Islands</t>
         </is>
       </c>
     </row>
@@ -32843,7 +32843,7 @@
       </c>
       <c r="F1179" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>
@@ -37445,7 +37445,7 @@
       </c>
       <c r="F1356" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Czechia</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ONEcampaign/aftershocks_data@3b52b413e6c4012c548f10ccd184119d263de3ee 🚀
</commit_message>
<xml_diff>
--- a/explorers/econ_metadata.xlsx
+++ b/explorers/econ_metadata.xlsx
@@ -25196,7 +25196,7 @@
         </is>
       </c>
       <c r="B885" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C885" t="inlineStr">
         <is>
@@ -25222,7 +25222,7 @@
         </is>
       </c>
       <c r="B886" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C886" t="inlineStr">
         <is>
@@ -25248,7 +25248,7 @@
         </is>
       </c>
       <c r="B887" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C887" t="inlineStr">
         <is>
@@ -25274,7 +25274,7 @@
         </is>
       </c>
       <c r="B888" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C888" t="inlineStr">
         <is>
@@ -25300,7 +25300,7 @@
         </is>
       </c>
       <c r="B889" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C889" t="inlineStr">
         <is>
@@ -25326,7 +25326,7 @@
         </is>
       </c>
       <c r="B890" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C890" t="inlineStr">
         <is>
@@ -25352,7 +25352,7 @@
         </is>
       </c>
       <c r="B891" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C891" t="inlineStr">
         <is>
@@ -25378,7 +25378,7 @@
         </is>
       </c>
       <c r="B892" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C892" t="inlineStr">
         <is>
@@ -25404,7 +25404,7 @@
         </is>
       </c>
       <c r="B893" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C893" t="inlineStr">
         <is>
@@ -25430,7 +25430,7 @@
         </is>
       </c>
       <c r="B894" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C894" t="inlineStr">
         <is>
@@ -25456,7 +25456,7 @@
         </is>
       </c>
       <c r="B895" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C895" t="inlineStr">
         <is>
@@ -25482,7 +25482,7 @@
         </is>
       </c>
       <c r="B896" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C896" t="inlineStr">
         <is>
@@ -25508,7 +25508,7 @@
         </is>
       </c>
       <c r="B897" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C897" t="inlineStr">
         <is>
@@ -25534,7 +25534,7 @@
         </is>
       </c>
       <c r="B898" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C898" t="inlineStr">
         <is>
@@ -25560,7 +25560,7 @@
         </is>
       </c>
       <c r="B899" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C899" t="inlineStr">
         <is>
@@ -25586,7 +25586,7 @@
         </is>
       </c>
       <c r="B900" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C900" t="inlineStr">
         <is>
@@ -25612,7 +25612,7 @@
         </is>
       </c>
       <c r="B901" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C901" t="inlineStr">
         <is>
@@ -25638,7 +25638,7 @@
         </is>
       </c>
       <c r="B902" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C902" t="inlineStr">
         <is>
@@ -25664,7 +25664,7 @@
         </is>
       </c>
       <c r="B903" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C903" t="inlineStr">
         <is>
@@ -25690,7 +25690,7 @@
         </is>
       </c>
       <c r="B904" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C904" t="inlineStr">
         <is>
@@ -25716,7 +25716,7 @@
         </is>
       </c>
       <c r="B905" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C905" t="inlineStr">
         <is>
@@ -25742,7 +25742,7 @@
         </is>
       </c>
       <c r="B906" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C906" t="inlineStr">
         <is>
@@ -25768,7 +25768,7 @@
         </is>
       </c>
       <c r="B907" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C907" t="inlineStr">
         <is>
@@ -25794,7 +25794,7 @@
         </is>
       </c>
       <c r="B908" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C908" t="inlineStr">
         <is>
@@ -25820,7 +25820,7 @@
         </is>
       </c>
       <c r="B909" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C909" t="inlineStr">
         <is>
@@ -25846,7 +25846,7 @@
         </is>
       </c>
       <c r="B910" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C910" t="inlineStr">
         <is>
@@ -25872,7 +25872,7 @@
         </is>
       </c>
       <c r="B911" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C911" t="inlineStr">
         <is>
@@ -25898,7 +25898,7 @@
         </is>
       </c>
       <c r="B912" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C912" t="inlineStr">
         <is>
@@ -25924,7 +25924,7 @@
         </is>
       </c>
       <c r="B913" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C913" t="inlineStr">
         <is>
@@ -25950,7 +25950,7 @@
         </is>
       </c>
       <c r="B914" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C914" t="inlineStr">
         <is>
@@ -25976,7 +25976,7 @@
         </is>
       </c>
       <c r="B915" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C915" t="inlineStr">
         <is>
@@ -26002,7 +26002,7 @@
         </is>
       </c>
       <c r="B916" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C916" t="inlineStr">
         <is>
@@ -26028,7 +26028,7 @@
         </is>
       </c>
       <c r="B917" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C917" t="inlineStr">
         <is>
@@ -26054,7 +26054,7 @@
         </is>
       </c>
       <c r="B918" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C918" t="inlineStr">
         <is>
@@ -26080,7 +26080,7 @@
         </is>
       </c>
       <c r="B919" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C919" t="inlineStr">
         <is>
@@ -26106,7 +26106,7 @@
         </is>
       </c>
       <c r="B920" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C920" t="inlineStr">
         <is>
@@ -26132,7 +26132,7 @@
         </is>
       </c>
       <c r="B921" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C921" t="inlineStr">
         <is>
@@ -26158,7 +26158,7 @@
         </is>
       </c>
       <c r="B922" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C922" t="inlineStr">
         <is>
@@ -26184,7 +26184,7 @@
         </is>
       </c>
       <c r="B923" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C923" t="inlineStr">
         <is>
@@ -26210,7 +26210,7 @@
         </is>
       </c>
       <c r="B924" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C924" t="inlineStr">
         <is>
@@ -26236,7 +26236,7 @@
         </is>
       </c>
       <c r="B925" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C925" t="inlineStr">
         <is>
@@ -26262,7 +26262,7 @@
         </is>
       </c>
       <c r="B926" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C926" t="inlineStr">
         <is>
@@ -26288,7 +26288,7 @@
         </is>
       </c>
       <c r="B927" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C927" t="inlineStr">
         <is>
@@ -26314,7 +26314,7 @@
         </is>
       </c>
       <c r="B928" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C928" t="inlineStr">
         <is>
@@ -26340,7 +26340,7 @@
         </is>
       </c>
       <c r="B929" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C929" t="inlineStr">
         <is>
@@ -26366,7 +26366,7 @@
         </is>
       </c>
       <c r="B930" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C930" t="inlineStr">
         <is>
@@ -26392,7 +26392,7 @@
         </is>
       </c>
       <c r="B931" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C931" t="inlineStr">
         <is>
@@ -26418,7 +26418,7 @@
         </is>
       </c>
       <c r="B932" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C932" t="inlineStr">
         <is>
@@ -26444,7 +26444,7 @@
         </is>
       </c>
       <c r="B933" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C933" t="inlineStr">
         <is>
@@ -26470,7 +26470,7 @@
         </is>
       </c>
       <c r="B934" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C934" t="inlineStr">
         <is>
@@ -26496,7 +26496,7 @@
         </is>
       </c>
       <c r="B935" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C935" t="inlineStr">
         <is>
@@ -26522,7 +26522,7 @@
         </is>
       </c>
       <c r="B936" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C936" t="inlineStr">
         <is>
@@ -26548,7 +26548,7 @@
         </is>
       </c>
       <c r="B937" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C937" t="inlineStr">
         <is>
@@ -26574,7 +26574,7 @@
         </is>
       </c>
       <c r="B938" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C938" t="inlineStr">
         <is>
@@ -26600,7 +26600,7 @@
         </is>
       </c>
       <c r="B939" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C939" t="inlineStr">
         <is>
@@ -26626,7 +26626,7 @@
         </is>
       </c>
       <c r="B940" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C940" t="inlineStr">
         <is>
@@ -26652,7 +26652,7 @@
         </is>
       </c>
       <c r="B941" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C941" t="inlineStr">
         <is>
@@ -26678,7 +26678,7 @@
         </is>
       </c>
       <c r="B942" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C942" t="inlineStr">
         <is>
@@ -26704,7 +26704,7 @@
         </is>
       </c>
       <c r="B943" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C943" t="inlineStr">
         <is>
@@ -26730,7 +26730,7 @@
         </is>
       </c>
       <c r="B944" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C944" t="inlineStr">
         <is>
@@ -26756,7 +26756,7 @@
         </is>
       </c>
       <c r="B945" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C945" t="inlineStr">
         <is>
@@ -26782,7 +26782,7 @@
         </is>
       </c>
       <c r="B946" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C946" t="inlineStr">
         <is>
@@ -26808,7 +26808,7 @@
         </is>
       </c>
       <c r="B947" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C947" t="inlineStr">
         <is>
@@ -26834,7 +26834,7 @@
         </is>
       </c>
       <c r="B948" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C948" t="inlineStr">
         <is>
@@ -26860,7 +26860,7 @@
         </is>
       </c>
       <c r="B949" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C949" t="inlineStr">
         <is>
@@ -26886,7 +26886,7 @@
         </is>
       </c>
       <c r="B950" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C950" t="inlineStr">
         <is>
@@ -26912,7 +26912,7 @@
         </is>
       </c>
       <c r="B951" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C951" t="inlineStr">
         <is>
@@ -26938,7 +26938,7 @@
         </is>
       </c>
       <c r="B952" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C952" t="inlineStr">
         <is>
@@ -26964,7 +26964,7 @@
         </is>
       </c>
       <c r="B953" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C953" t="inlineStr">
         <is>
@@ -26990,7 +26990,7 @@
         </is>
       </c>
       <c r="B954" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C954" t="inlineStr">
         <is>
@@ -27016,7 +27016,7 @@
         </is>
       </c>
       <c r="B955" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C955" t="inlineStr">
         <is>
@@ -27042,7 +27042,7 @@
         </is>
       </c>
       <c r="B956" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C956" t="inlineStr">
         <is>
@@ -27068,7 +27068,7 @@
         </is>
       </c>
       <c r="B957" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C957" t="inlineStr">
         <is>
@@ -27094,7 +27094,7 @@
         </is>
       </c>
       <c r="B958" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C958" t="inlineStr">
         <is>
@@ -27120,7 +27120,7 @@
         </is>
       </c>
       <c r="B959" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C959" t="inlineStr">
         <is>
@@ -27146,7 +27146,7 @@
         </is>
       </c>
       <c r="B960" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C960" t="inlineStr">
         <is>
@@ -27172,7 +27172,7 @@
         </is>
       </c>
       <c r="B961" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C961" t="inlineStr">
         <is>
@@ -27198,7 +27198,7 @@
         </is>
       </c>
       <c r="B962" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C962" t="inlineStr">
         <is>
@@ -27224,7 +27224,7 @@
         </is>
       </c>
       <c r="B963" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C963" t="inlineStr">
         <is>
@@ -27250,7 +27250,7 @@
         </is>
       </c>
       <c r="B964" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C964" t="inlineStr">
         <is>
@@ -27276,7 +27276,7 @@
         </is>
       </c>
       <c r="B965" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C965" t="inlineStr">
         <is>
@@ -27302,7 +27302,7 @@
         </is>
       </c>
       <c r="B966" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C966" t="inlineStr">
         <is>
@@ -27328,7 +27328,7 @@
         </is>
       </c>
       <c r="B967" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C967" t="inlineStr">
         <is>
@@ -27354,7 +27354,7 @@
         </is>
       </c>
       <c r="B968" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C968" t="inlineStr">
         <is>
@@ -27380,7 +27380,7 @@
         </is>
       </c>
       <c r="B969" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C969" t="inlineStr">
         <is>
@@ -27406,7 +27406,7 @@
         </is>
       </c>
       <c r="B970" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C970" t="inlineStr">
         <is>
@@ -27432,7 +27432,7 @@
         </is>
       </c>
       <c r="B971" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C971" t="inlineStr">
         <is>
@@ -27458,7 +27458,7 @@
         </is>
       </c>
       <c r="B972" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C972" t="inlineStr">
         <is>
@@ -27484,7 +27484,7 @@
         </is>
       </c>
       <c r="B973" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C973" t="inlineStr">
         <is>
@@ -27510,7 +27510,7 @@
         </is>
       </c>
       <c r="B974" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C974" t="inlineStr">
         <is>
@@ -27536,7 +27536,7 @@
         </is>
       </c>
       <c r="B975" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C975" t="inlineStr">
         <is>
@@ -27562,7 +27562,7 @@
         </is>
       </c>
       <c r="B976" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C976" t="inlineStr">
         <is>
@@ -27588,7 +27588,7 @@
         </is>
       </c>
       <c r="B977" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C977" t="inlineStr">
         <is>
@@ -27614,7 +27614,7 @@
         </is>
       </c>
       <c r="B978" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C978" t="inlineStr">
         <is>
@@ -27640,7 +27640,7 @@
         </is>
       </c>
       <c r="B979" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C979" t="inlineStr">
         <is>
@@ -27666,7 +27666,7 @@
         </is>
       </c>
       <c r="B980" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C980" t="inlineStr">
         <is>
@@ -27692,7 +27692,7 @@
         </is>
       </c>
       <c r="B981" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C981" t="inlineStr">
         <is>
@@ -27718,7 +27718,7 @@
         </is>
       </c>
       <c r="B982" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C982" t="inlineStr">
         <is>
@@ -27744,7 +27744,7 @@
         </is>
       </c>
       <c r="B983" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C983" t="inlineStr">
         <is>
@@ -27770,7 +27770,7 @@
         </is>
       </c>
       <c r="B984" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C984" t="inlineStr">
         <is>
@@ -27796,7 +27796,7 @@
         </is>
       </c>
       <c r="B985" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C985" t="inlineStr">
         <is>
@@ -27822,7 +27822,7 @@
         </is>
       </c>
       <c r="B986" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C986" t="inlineStr">
         <is>
@@ -27848,7 +27848,7 @@
         </is>
       </c>
       <c r="B987" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C987" t="inlineStr">
         <is>
@@ -27874,7 +27874,7 @@
         </is>
       </c>
       <c r="B988" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C988" t="inlineStr">
         <is>
@@ -27900,7 +27900,7 @@
         </is>
       </c>
       <c r="B989" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C989" t="inlineStr">
         <is>
@@ -27926,7 +27926,7 @@
         </is>
       </c>
       <c r="B990" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C990" t="inlineStr">
         <is>
@@ -27952,7 +27952,7 @@
         </is>
       </c>
       <c r="B991" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C991" t="inlineStr">
         <is>
@@ -27978,7 +27978,7 @@
         </is>
       </c>
       <c r="B992" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C992" t="inlineStr">
         <is>
@@ -28004,7 +28004,7 @@
         </is>
       </c>
       <c r="B993" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C993" t="inlineStr">
         <is>
@@ -28030,7 +28030,7 @@
         </is>
       </c>
       <c r="B994" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C994" t="inlineStr">
         <is>
@@ -28056,7 +28056,7 @@
         </is>
       </c>
       <c r="B995" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C995" t="inlineStr">
         <is>
@@ -28082,7 +28082,7 @@
         </is>
       </c>
       <c r="B996" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C996" t="inlineStr">
         <is>
@@ -28108,7 +28108,7 @@
         </is>
       </c>
       <c r="B997" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C997" t="inlineStr">
         <is>
@@ -28134,7 +28134,7 @@
         </is>
       </c>
       <c r="B998" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C998" t="inlineStr">
         <is>
@@ -28160,7 +28160,7 @@
         </is>
       </c>
       <c r="B999" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C999" t="inlineStr">
         <is>
@@ -28186,7 +28186,7 @@
         </is>
       </c>
       <c r="B1000" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1000" t="inlineStr">
         <is>
@@ -28212,7 +28212,7 @@
         </is>
       </c>
       <c r="B1001" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1001" t="inlineStr">
         <is>
@@ -28238,7 +28238,7 @@
         </is>
       </c>
       <c r="B1002" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1002" t="inlineStr">
         <is>
@@ -28264,7 +28264,7 @@
         </is>
       </c>
       <c r="B1003" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1003" t="inlineStr">
         <is>
@@ -28290,7 +28290,7 @@
         </is>
       </c>
       <c r="B1004" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1004" t="inlineStr">
         <is>
@@ -28316,7 +28316,7 @@
         </is>
       </c>
       <c r="B1005" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1005" t="inlineStr">
         <is>
@@ -28342,7 +28342,7 @@
         </is>
       </c>
       <c r="B1006" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1006" t="inlineStr">
         <is>
@@ -28368,7 +28368,7 @@
         </is>
       </c>
       <c r="B1007" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1007" t="inlineStr">
         <is>
@@ -28394,7 +28394,7 @@
         </is>
       </c>
       <c r="B1008" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1008" t="inlineStr">
         <is>
@@ -28420,7 +28420,7 @@
         </is>
       </c>
       <c r="B1009" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1009" t="inlineStr">
         <is>
@@ -28446,7 +28446,7 @@
         </is>
       </c>
       <c r="B1010" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1010" t="inlineStr">
         <is>
@@ -28472,7 +28472,7 @@
         </is>
       </c>
       <c r="B1011" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1011" t="inlineStr">
         <is>
@@ -28498,7 +28498,7 @@
         </is>
       </c>
       <c r="B1012" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1012" t="inlineStr">
         <is>
@@ -28524,7 +28524,7 @@
         </is>
       </c>
       <c r="B1013" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1013" t="inlineStr">
         <is>
@@ -28550,7 +28550,7 @@
         </is>
       </c>
       <c r="B1014" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1014" t="inlineStr">
         <is>
@@ -28576,7 +28576,7 @@
         </is>
       </c>
       <c r="B1015" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1015" t="inlineStr">
         <is>
@@ -28602,7 +28602,7 @@
         </is>
       </c>
       <c r="B1016" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1016" t="inlineStr">
         <is>
@@ -28628,7 +28628,7 @@
         </is>
       </c>
       <c r="B1017" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1017" t="inlineStr">
         <is>
@@ -28654,7 +28654,7 @@
         </is>
       </c>
       <c r="B1018" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1018" t="inlineStr">
         <is>
@@ -28680,7 +28680,7 @@
         </is>
       </c>
       <c r="B1019" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1019" t="inlineStr">
         <is>
@@ -28706,7 +28706,7 @@
         </is>
       </c>
       <c r="B1020" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1020" t="inlineStr">
         <is>
@@ -28732,7 +28732,7 @@
         </is>
       </c>
       <c r="B1021" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1021" t="inlineStr">
         <is>
@@ -28758,7 +28758,7 @@
         </is>
       </c>
       <c r="B1022" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1022" t="inlineStr">
         <is>
@@ -28784,7 +28784,7 @@
         </is>
       </c>
       <c r="B1023" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1023" t="inlineStr">
         <is>
@@ -28810,7 +28810,7 @@
         </is>
       </c>
       <c r="B1024" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1024" t="inlineStr">
         <is>
@@ -28836,7 +28836,7 @@
         </is>
       </c>
       <c r="B1025" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1025" t="inlineStr">
         <is>
@@ -28862,7 +28862,7 @@
         </is>
       </c>
       <c r="B1026" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1026" t="inlineStr">
         <is>
@@ -28888,7 +28888,7 @@
         </is>
       </c>
       <c r="B1027" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1027" t="inlineStr">
         <is>
@@ -28914,7 +28914,7 @@
         </is>
       </c>
       <c r="B1028" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1028" t="inlineStr">
         <is>
@@ -28940,7 +28940,7 @@
         </is>
       </c>
       <c r="B1029" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1029" t="inlineStr">
         <is>
@@ -28966,7 +28966,7 @@
         </is>
       </c>
       <c r="B1030" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1030" t="inlineStr">
         <is>
@@ -28992,7 +28992,7 @@
         </is>
       </c>
       <c r="B1031" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1031" t="inlineStr">
         <is>
@@ -29018,7 +29018,7 @@
         </is>
       </c>
       <c r="B1032" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1032" t="inlineStr">
         <is>
@@ -29044,7 +29044,7 @@
         </is>
       </c>
       <c r="B1033" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1033" t="inlineStr">
         <is>
@@ -29070,7 +29070,7 @@
         </is>
       </c>
       <c r="B1034" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1034" t="inlineStr">
         <is>
@@ -29096,7 +29096,7 @@
         </is>
       </c>
       <c r="B1035" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1035" t="inlineStr">
         <is>
@@ -29122,7 +29122,7 @@
         </is>
       </c>
       <c r="B1036" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1036" t="inlineStr">
         <is>
@@ -29148,7 +29148,7 @@
         </is>
       </c>
       <c r="B1037" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1037" t="inlineStr">
         <is>
@@ -29174,7 +29174,7 @@
         </is>
       </c>
       <c r="B1038" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1038" t="inlineStr">
         <is>
@@ -29200,7 +29200,7 @@
         </is>
       </c>
       <c r="B1039" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1039" t="inlineStr">
         <is>
@@ -29226,7 +29226,7 @@
         </is>
       </c>
       <c r="B1040" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1040" t="inlineStr">
         <is>
@@ -29252,7 +29252,7 @@
         </is>
       </c>
       <c r="B1041" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1041" t="inlineStr">
         <is>
@@ -29278,7 +29278,7 @@
         </is>
       </c>
       <c r="B1042" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1042" t="inlineStr">
         <is>
@@ -29304,7 +29304,7 @@
         </is>
       </c>
       <c r="B1043" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1043" t="inlineStr">
         <is>
@@ -29330,7 +29330,7 @@
         </is>
       </c>
       <c r="B1044" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1044" t="inlineStr">
         <is>
@@ -29356,7 +29356,7 @@
         </is>
       </c>
       <c r="B1045" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1045" t="inlineStr">
         <is>
@@ -29382,7 +29382,7 @@
         </is>
       </c>
       <c r="B1046" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1046" t="inlineStr">
         <is>
@@ -29408,7 +29408,7 @@
         </is>
       </c>
       <c r="B1047" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1047" t="inlineStr">
         <is>
@@ -29434,7 +29434,7 @@
         </is>
       </c>
       <c r="B1048" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1048" t="inlineStr">
         <is>
@@ -29460,7 +29460,7 @@
         </is>
       </c>
       <c r="B1049" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1049" t="inlineStr">
         <is>
@@ -29486,7 +29486,7 @@
         </is>
       </c>
       <c r="B1050" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1050" t="inlineStr">
         <is>
@@ -29512,7 +29512,7 @@
         </is>
       </c>
       <c r="B1051" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1051" t="inlineStr">
         <is>
@@ -29538,7 +29538,7 @@
         </is>
       </c>
       <c r="B1052" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1052" t="inlineStr">
         <is>
@@ -29564,7 +29564,7 @@
         </is>
       </c>
       <c r="B1053" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1053" t="inlineStr">
         <is>
@@ -29590,7 +29590,7 @@
         </is>
       </c>
       <c r="B1054" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1054" t="inlineStr">
         <is>
@@ -29616,7 +29616,7 @@
         </is>
       </c>
       <c r="B1055" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1055" t="inlineStr">
         <is>
@@ -29642,7 +29642,7 @@
         </is>
       </c>
       <c r="B1056" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1056" t="inlineStr">
         <is>
@@ -29668,7 +29668,7 @@
         </is>
       </c>
       <c r="B1057" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1057" t="inlineStr">
         <is>
@@ -29694,7 +29694,7 @@
         </is>
       </c>
       <c r="B1058" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1058" t="inlineStr">
         <is>
@@ -29720,7 +29720,7 @@
         </is>
       </c>
       <c r="B1059" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1059" t="inlineStr">
         <is>
@@ -29746,7 +29746,7 @@
         </is>
       </c>
       <c r="B1060" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1060" t="inlineStr">
         <is>
@@ -29772,7 +29772,7 @@
         </is>
       </c>
       <c r="B1061" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1061" t="inlineStr">
         <is>
@@ -29798,7 +29798,7 @@
         </is>
       </c>
       <c r="B1062" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1062" t="inlineStr">
         <is>
@@ -29824,7 +29824,7 @@
         </is>
       </c>
       <c r="B1063" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1063" t="inlineStr">
         <is>
@@ -29850,7 +29850,7 @@
         </is>
       </c>
       <c r="B1064" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1064" t="inlineStr">
         <is>
@@ -29876,7 +29876,7 @@
         </is>
       </c>
       <c r="B1065" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1065" t="inlineStr">
         <is>
@@ -29902,7 +29902,7 @@
         </is>
       </c>
       <c r="B1066" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1066" t="inlineStr">
         <is>
@@ -29928,7 +29928,7 @@
         </is>
       </c>
       <c r="B1067" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1067" t="inlineStr">
         <is>
@@ -29954,7 +29954,7 @@
         </is>
       </c>
       <c r="B1068" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1068" t="inlineStr">
         <is>
@@ -29980,7 +29980,7 @@
         </is>
       </c>
       <c r="B1069" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1069" t="inlineStr">
         <is>
@@ -30006,7 +30006,7 @@
         </is>
       </c>
       <c r="B1070" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1070" t="inlineStr">
         <is>
@@ -30032,7 +30032,7 @@
         </is>
       </c>
       <c r="B1071" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1071" t="inlineStr">
         <is>
@@ -30058,7 +30058,7 @@
         </is>
       </c>
       <c r="B1072" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1072" t="inlineStr">
         <is>
@@ -30084,7 +30084,7 @@
         </is>
       </c>
       <c r="B1073" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1073" t="inlineStr">
         <is>
@@ -30110,7 +30110,7 @@
         </is>
       </c>
       <c r="B1074" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1074" t="inlineStr">
         <is>
@@ -30136,7 +30136,7 @@
         </is>
       </c>
       <c r="B1075" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1075" t="inlineStr">
         <is>
@@ -30162,7 +30162,7 @@
         </is>
       </c>
       <c r="B1076" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1076" t="inlineStr">
         <is>
@@ -30188,7 +30188,7 @@
         </is>
       </c>
       <c r="B1077" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1077" t="inlineStr">
         <is>
@@ -30214,7 +30214,7 @@
         </is>
       </c>
       <c r="B1078" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1078" t="inlineStr">
         <is>
@@ -30240,7 +30240,7 @@
         </is>
       </c>
       <c r="B1079" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1079" t="inlineStr">
         <is>
@@ -30266,7 +30266,7 @@
         </is>
       </c>
       <c r="B1080" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1080" t="inlineStr">
         <is>
@@ -30292,7 +30292,7 @@
         </is>
       </c>
       <c r="B1081" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1081" t="inlineStr">
         <is>
@@ -30318,7 +30318,7 @@
         </is>
       </c>
       <c r="B1082" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1082" t="inlineStr">
         <is>
@@ -30344,7 +30344,7 @@
         </is>
       </c>
       <c r="B1083" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1083" t="inlineStr">
         <is>
@@ -30370,7 +30370,7 @@
         </is>
       </c>
       <c r="B1084" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1084" t="inlineStr">
         <is>
@@ -30396,7 +30396,7 @@
         </is>
       </c>
       <c r="B1085" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1085" t="inlineStr">
         <is>
@@ -30422,7 +30422,7 @@
         </is>
       </c>
       <c r="B1086" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1086" t="inlineStr">
         <is>
@@ -30448,7 +30448,7 @@
         </is>
       </c>
       <c r="B1087" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1087" t="inlineStr">
         <is>
@@ -30474,7 +30474,7 @@
         </is>
       </c>
       <c r="B1088" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1088" t="inlineStr">
         <is>
@@ -30500,7 +30500,7 @@
         </is>
       </c>
       <c r="B1089" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1089" t="inlineStr">
         <is>
@@ -30526,7 +30526,7 @@
         </is>
       </c>
       <c r="B1090" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1090" t="inlineStr">
         <is>
@@ -30552,7 +30552,7 @@
         </is>
       </c>
       <c r="B1091" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1091" t="inlineStr">
         <is>
@@ -30578,7 +30578,7 @@
         </is>
       </c>
       <c r="B1092" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1092" t="inlineStr">
         <is>
@@ -30604,7 +30604,7 @@
         </is>
       </c>
       <c r="B1093" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1093" t="inlineStr">
         <is>
@@ -30630,7 +30630,7 @@
         </is>
       </c>
       <c r="B1094" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1094" t="inlineStr">
         <is>
@@ -30656,7 +30656,7 @@
         </is>
       </c>
       <c r="B1095" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1095" t="inlineStr">
         <is>
@@ -30682,7 +30682,7 @@
         </is>
       </c>
       <c r="B1096" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1096" t="inlineStr">
         <is>
@@ -30708,7 +30708,7 @@
         </is>
       </c>
       <c r="B1097" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1097" t="inlineStr">
         <is>
@@ -30734,7 +30734,7 @@
         </is>
       </c>
       <c r="B1098" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1098" t="inlineStr">
         <is>
@@ -30760,7 +30760,7 @@
         </is>
       </c>
       <c r="B1099" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1099" t="inlineStr">
         <is>
@@ -30786,7 +30786,7 @@
         </is>
       </c>
       <c r="B1100" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1100" t="inlineStr">
         <is>
@@ -30812,7 +30812,7 @@
         </is>
       </c>
       <c r="B1101" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1101" t="inlineStr">
         <is>
@@ -30838,7 +30838,7 @@
         </is>
       </c>
       <c r="B1102" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1102" t="inlineStr">
         <is>
@@ -30864,7 +30864,7 @@
         </is>
       </c>
       <c r="B1103" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1103" t="inlineStr">
         <is>
@@ -30890,7 +30890,7 @@
         </is>
       </c>
       <c r="B1104" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1104" t="inlineStr">
         <is>
@@ -30916,7 +30916,7 @@
         </is>
       </c>
       <c r="B1105" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1105" t="inlineStr">
         <is>
@@ -30942,7 +30942,7 @@
         </is>
       </c>
       <c r="B1106" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1106" t="inlineStr">
         <is>
@@ -30968,7 +30968,7 @@
         </is>
       </c>
       <c r="B1107" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1107" t="inlineStr">
         <is>
@@ -30994,7 +30994,7 @@
         </is>
       </c>
       <c r="B1108" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1108" t="inlineStr">
         <is>
@@ -31020,7 +31020,7 @@
         </is>
       </c>
       <c r="B1109" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1109" t="inlineStr">
         <is>
@@ -31046,7 +31046,7 @@
         </is>
       </c>
       <c r="B1110" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1110" t="inlineStr">
         <is>
@@ -31072,7 +31072,7 @@
         </is>
       </c>
       <c r="B1111" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1111" t="inlineStr">
         <is>
@@ -31098,7 +31098,7 @@
         </is>
       </c>
       <c r="B1112" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1112" t="inlineStr">
         <is>
@@ -31124,7 +31124,7 @@
         </is>
       </c>
       <c r="B1113" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1113" t="inlineStr">
         <is>
@@ -31150,7 +31150,7 @@
         </is>
       </c>
       <c r="B1114" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1114" t="inlineStr">
         <is>
@@ -31176,7 +31176,7 @@
         </is>
       </c>
       <c r="B1115" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1115" t="inlineStr">
         <is>
@@ -31202,7 +31202,7 @@
         </is>
       </c>
       <c r="B1116" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1116" t="inlineStr">
         <is>
@@ -31228,7 +31228,7 @@
         </is>
       </c>
       <c r="B1117" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1117" t="inlineStr">
         <is>
@@ -31254,7 +31254,7 @@
         </is>
       </c>
       <c r="B1118" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1118" t="inlineStr">
         <is>
@@ -31280,7 +31280,7 @@
         </is>
       </c>
       <c r="B1119" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1119" t="inlineStr">
         <is>
@@ -31306,7 +31306,7 @@
         </is>
       </c>
       <c r="B1120" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1120" t="inlineStr">
         <is>
@@ -31332,7 +31332,7 @@
         </is>
       </c>
       <c r="B1121" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1121" t="inlineStr">
         <is>
@@ -31358,7 +31358,7 @@
         </is>
       </c>
       <c r="B1122" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1122" t="inlineStr">
         <is>
@@ -31384,7 +31384,7 @@
         </is>
       </c>
       <c r="B1123" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1123" t="inlineStr">
         <is>
@@ -31410,7 +31410,7 @@
         </is>
       </c>
       <c r="B1124" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1124" t="inlineStr">
         <is>
@@ -31436,7 +31436,7 @@
         </is>
       </c>
       <c r="B1125" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1125" t="inlineStr">
         <is>
@@ -31462,7 +31462,7 @@
         </is>
       </c>
       <c r="B1126" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1126" t="inlineStr">
         <is>
@@ -31488,7 +31488,7 @@
         </is>
       </c>
       <c r="B1127" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1127" t="inlineStr">
         <is>
@@ -31514,7 +31514,7 @@
         </is>
       </c>
       <c r="B1128" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1128" t="inlineStr">
         <is>
@@ -31540,7 +31540,7 @@
         </is>
       </c>
       <c r="B1129" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1129" t="inlineStr">
         <is>
@@ -31566,7 +31566,7 @@
         </is>
       </c>
       <c r="B1130" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1130" t="inlineStr">
         <is>
@@ -31592,7 +31592,7 @@
         </is>
       </c>
       <c r="B1131" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1131" t="inlineStr">
         <is>
@@ -31618,7 +31618,7 @@
         </is>
       </c>
       <c r="B1132" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1132" t="inlineStr">
         <is>
@@ -31644,7 +31644,7 @@
         </is>
       </c>
       <c r="B1133" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1133" t="inlineStr">
         <is>
@@ -31670,7 +31670,7 @@
         </is>
       </c>
       <c r="B1134" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1134" t="inlineStr">
         <is>
@@ -31696,7 +31696,7 @@
         </is>
       </c>
       <c r="B1135" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1135" t="inlineStr">
         <is>
@@ -31722,7 +31722,7 @@
         </is>
       </c>
       <c r="B1136" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1136" t="inlineStr">
         <is>
@@ -31748,7 +31748,7 @@
         </is>
       </c>
       <c r="B1137" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1137" t="inlineStr">
         <is>
@@ -31774,7 +31774,7 @@
         </is>
       </c>
       <c r="B1138" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1138" t="inlineStr">
         <is>
@@ -31800,7 +31800,7 @@
         </is>
       </c>
       <c r="B1139" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1139" t="inlineStr">
         <is>
@@ -31826,7 +31826,7 @@
         </is>
       </c>
       <c r="B1140" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1140" t="inlineStr">
         <is>
@@ -31852,7 +31852,7 @@
         </is>
       </c>
       <c r="B1141" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1141" t="inlineStr">
         <is>
@@ -31878,7 +31878,7 @@
         </is>
       </c>
       <c r="B1142" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1142" t="inlineStr">
         <is>
@@ -31904,7 +31904,7 @@
         </is>
       </c>
       <c r="B1143" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1143" t="inlineStr">
         <is>
@@ -31930,7 +31930,7 @@
         </is>
       </c>
       <c r="B1144" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1144" t="inlineStr">
         <is>
@@ -31956,7 +31956,7 @@
         </is>
       </c>
       <c r="B1145" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1145" t="inlineStr">
         <is>
@@ -31982,7 +31982,7 @@
         </is>
       </c>
       <c r="B1146" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1146" t="inlineStr">
         <is>
@@ -32008,7 +32008,7 @@
         </is>
       </c>
       <c r="B1147" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1147" t="inlineStr">
         <is>
@@ -32034,7 +32034,7 @@
         </is>
       </c>
       <c r="B1148" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1148" t="inlineStr">
         <is>
@@ -32060,7 +32060,7 @@
         </is>
       </c>
       <c r="B1149" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C1149" t="inlineStr">
         <is>

</xml_diff>